<commit_message>
added potential output and NAIRU for DK + unemployment rate gap
</commit_message>
<xml_diff>
--- a/data/monaData.xlsx
+++ b/data/monaData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\srv9dnbfil002\userhome\cjw\Documents\Inflation cluster\Semi-structurcal model of inflation dynamics\Data\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB7DEBA5-3142-4685-B995-9515A02006B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E17572-3091-422F-B6DA-B78C397C9718}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11010" xr2:uid="{3893118A-CCCC-4227-9FE2-63195E760603}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 refTo: string
 refFreq: string
 BankPath: g:\mona\gekko30\prbanker\pr2203.gbk
-Series: fy, fy_gab, qby, praoli, pcpdkeu
+Series: fy, fy_gab, qby, praoli, pcpdkeu, ulb2, u2, u2_str, ulb2_str, fy_str
 StartPeriod: 1999
 EndPeriod: 2022
 Frequency: q
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
   <si>
     <t>fy_gab</t>
   </si>
@@ -363,6 +363,30 @@
   </si>
   <si>
     <t>pcpdkeu</t>
+  </si>
+  <si>
+    <t>u2</t>
+  </si>
+  <si>
+    <t>ulb2</t>
+  </si>
+  <si>
+    <t>u2_str</t>
+  </si>
+  <si>
+    <t>ulb2_str</t>
+  </si>
+  <si>
+    <t>ur</t>
+  </si>
+  <si>
+    <t>ur_str</t>
+  </si>
+  <si>
+    <t>ur_gab</t>
+  </si>
+  <si>
+    <t>fy_str</t>
   </si>
 </sst>
 </file>
@@ -720,13 +744,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B36B7F14-513A-48A1-91F4-A424ABF8C6B9}">
-  <dimension ref="A1:F97"/>
+  <dimension ref="A1:N97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>97</v>
       </c>
@@ -742,8 +768,32 @@
       <c r="F1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L1" t="s">
+        <v>105</v>
+      </c>
+      <c r="M1" t="s">
+        <v>106</v>
+      </c>
+      <c r="N1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -762,8 +812,35 @@
       <c r="F2">
         <v>0.79299830000000004</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>184.24585999999999</v>
+      </c>
+      <c r="H2">
+        <v>2818.96486</v>
+      </c>
+      <c r="I2">
+        <v>2853.7617700000001</v>
+      </c>
+      <c r="J2">
+        <v>221.880044</v>
+      </c>
+      <c r="K2">
+        <v>1591.3602100000001</v>
+      </c>
+      <c r="L2">
+        <f>G2/H2*100</f>
+        <v>6.5359402883794733</v>
+      </c>
+      <c r="M2">
+        <f>J2/I2*100</f>
+        <v>7.7750023261402079</v>
+      </c>
+      <c r="N2">
+        <f>L2-M2</f>
+        <v>-1.2390620377607346</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -782,8 +859,35 @@
       <c r="F3">
         <v>0.79805919999999997</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>184.18314699999999</v>
+      </c>
+      <c r="H3">
+        <v>2814.78215</v>
+      </c>
+      <c r="I3">
+        <v>2854.7461400000002</v>
+      </c>
+      <c r="J3">
+        <v>218.89852999999999</v>
+      </c>
+      <c r="K3">
+        <v>1600.23684</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L66" si="0">G3/H3*100</f>
+        <v>6.5434245772803408</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M66" si="1">J3/I3*100</f>
+        <v>7.6678807594429381</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N66" si="2">L3-M3</f>
+        <v>-1.1244561821625974</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -802,8 +906,35 @@
       <c r="F4">
         <v>0.80463280000000004</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>182.533041</v>
+      </c>
+      <c r="H4">
+        <v>2824.8520400000002</v>
+      </c>
+      <c r="I4">
+        <v>2855.6819500000001</v>
+      </c>
+      <c r="J4">
+        <v>215.93140600000001</v>
+      </c>
+      <c r="K4">
+        <v>1608.94829</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>6.4616850162530977</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="1"/>
+        <v>7.5614655196458411</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="2"/>
+        <v>-1.0997805033927435</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -822,8 +953,35 @@
       <c r="F5">
         <v>0.81037269999999995</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>182.246883</v>
+      </c>
+      <c r="H5">
+        <v>2826.1518799999999</v>
+      </c>
+      <c r="I5">
+        <v>2856.4465</v>
+      </c>
+      <c r="J5">
+        <v>213.06732600000001</v>
+      </c>
+      <c r="K5">
+        <v>1618.1419699999999</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>6.4485877170904207</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="1"/>
+        <v>7.4591743972799769</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="2"/>
+        <v>-1.0105866801895562</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -842,8 +1000,35 @@
       <c r="F6">
         <v>0.81545609971177291</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>181.722791</v>
+      </c>
+      <c r="H6">
+        <v>2841.4554199999998</v>
+      </c>
+      <c r="I6">
+        <v>2862.3404500000001</v>
+      </c>
+      <c r="J6">
+        <v>210.62571399999999</v>
+      </c>
+      <c r="K6">
+        <v>1629.59681</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>6.3954123552640505</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="1"/>
+        <v>7.3585136946235723</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="2"/>
+        <v>-0.9631013393595218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -862,8 +1047,35 @@
       <c r="F7">
         <v>0.82076079743577601</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>178.80327</v>
+      </c>
+      <c r="H7">
+        <v>2832.9541399999998</v>
+      </c>
+      <c r="I7">
+        <v>2863.52279</v>
+      </c>
+      <c r="J7">
+        <v>207.86847299999999</v>
+      </c>
+      <c r="K7">
+        <v>1639.2682299999999</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>6.3115483401365617</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="1"/>
+        <v>7.2591869611067423</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="2"/>
+        <v>-0.94763862097018059</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -882,8 +1094,35 @@
       <c r="F8">
         <v>0.82526639679814651</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>176.42092199999999</v>
+      </c>
+      <c r="H8">
+        <v>2837.2400200000002</v>
+      </c>
+      <c r="I8">
+        <v>2864.6955600000001</v>
+      </c>
+      <c r="J8">
+        <v>205.147492</v>
+      </c>
+      <c r="K8">
+        <v>1648.3013599999999</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>6.2180471428709083</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="1"/>
+        <v>7.1612318902047649</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="2"/>
+        <v>-0.9431847473338566</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -902,8 +1141,35 @@
       <c r="F9">
         <v>0.83148990224916797</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>172.79444899999999</v>
+      </c>
+      <c r="H9">
+        <v>2833.5366399999998</v>
+      </c>
+      <c r="I9">
+        <v>2865.57566</v>
+      </c>
+      <c r="J9">
+        <v>202.42139299999999</v>
+      </c>
+      <c r="K9">
+        <v>1656.95759</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>6.0981900343452065</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="1"/>
+        <v>7.0638997889869009</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="2"/>
+        <v>-0.9657097546416944</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -922,8 +1188,35 @@
       <c r="F10">
         <v>0.8342586111019421</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>171.155349</v>
+      </c>
+      <c r="H10">
+        <v>2855.3015300000002</v>
+      </c>
+      <c r="I10">
+        <v>2867.1771600000002</v>
+      </c>
+      <c r="J10">
+        <v>199.78205600000001</v>
+      </c>
+      <c r="K10">
+        <v>1664.73524</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>5.9943003287642265</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="1"/>
+        <v>6.9679006511059125</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="2"/>
+        <v>-0.97360032234168603</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -942,8 +1235,35 @@
       <c r="F11">
         <v>0.84173352233877441</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>166.979198</v>
+      </c>
+      <c r="H11">
+        <v>2856.8195099999998</v>
+      </c>
+      <c r="I11">
+        <v>2869.0661399999999</v>
+      </c>
+      <c r="J11">
+        <v>197.16194400000001</v>
+      </c>
+      <c r="K11">
+        <v>1673.3064300000001</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>5.8449334098813965</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="1"/>
+        <v>6.8719902009648335</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="2"/>
+        <v>-1.0270567910834369</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -962,8 +1282,35 @@
       <c r="F12">
         <v>0.84470432981577814</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>164.178753</v>
+      </c>
+      <c r="H12">
+        <v>2846.2370900000001</v>
+      </c>
+      <c r="I12">
+        <v>2870.18345</v>
+      </c>
+      <c r="J12">
+        <v>194.56410399999999</v>
+      </c>
+      <c r="K12">
+        <v>1681.6279400000001</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>5.7682739634314864</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="1"/>
+        <v>6.7788037729783435</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="2"/>
+        <v>-1.0105298095468571</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -982,8 +1329,35 @@
       <c r="F13">
         <v>0.84801543833669291</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>162.18951100000001</v>
+      </c>
+      <c r="H13">
+        <v>2852.8621600000001</v>
+      </c>
+      <c r="I13">
+        <v>2872.9499500000002</v>
+      </c>
+      <c r="J13">
+        <v>192.11828800000001</v>
+      </c>
+      <c r="K13">
+        <v>1690.14058</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>5.6851506278172241</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="1"/>
+        <v>6.687143575195245</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="2"/>
+        <v>-1.0019929473780209</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1002,8 +1376,35 @@
       <c r="F14">
         <v>0.85435014950645172</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>165.998637</v>
+      </c>
+      <c r="H14">
+        <v>2855.0302999999999</v>
+      </c>
+      <c r="I14">
+        <v>2874.5660899999998</v>
+      </c>
+      <c r="J14">
+        <v>189.773551</v>
+      </c>
+      <c r="K14">
+        <v>1697.65814</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>5.8142513233572339</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="1"/>
+        <v>6.6018155456637988</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="2"/>
+        <v>-0.78756422230656487</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1022,8 +1423,35 @@
       <c r="F15">
         <v>0.85940465996177318</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>165.045727</v>
+      </c>
+      <c r="H15">
+        <v>2859.4812700000002</v>
+      </c>
+      <c r="I15">
+        <v>2874.7923099999998</v>
+      </c>
+      <c r="J15">
+        <v>187.291608</v>
+      </c>
+      <c r="K15">
+        <v>1704.0469700000001</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>5.7718764844366337</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="1"/>
+        <v>6.5149613538516808</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="2"/>
+        <v>-0.74308486941504714</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1042,8 +1470,35 @@
       <c r="F16">
         <v>0.86466367413584966</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>166.51862</v>
+      </c>
+      <c r="H16">
+        <v>2858.4651899999999</v>
+      </c>
+      <c r="I16">
+        <v>2876.0204699999999</v>
+      </c>
+      <c r="J16">
+        <v>184.98566299999999</v>
+      </c>
+      <c r="K16">
+        <v>1710.7340099999999</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>5.8254555830361534</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="1"/>
+        <v>6.4320009168780361</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="2"/>
+        <v>-0.60654533384188269</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1062,8 +1517,35 @@
       <c r="F17">
         <v>0.87054478753052278</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>169.93381600000001</v>
+      </c>
+      <c r="H17">
+        <v>2857.7744699999998</v>
+      </c>
+      <c r="I17">
+        <v>2876.2884399999998</v>
+      </c>
+      <c r="J17">
+        <v>182.70028300000001</v>
+      </c>
+      <c r="K17">
+        <v>1716.8100400000001</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>5.9463690289038107</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="1"/>
+        <v>6.3519458083279021</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="2"/>
+        <v>-0.40557677942409143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1082,8 +1564,35 @@
       <c r="F18">
         <v>0.87816629762936438</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>176.750427</v>
+      </c>
+      <c r="H18">
+        <v>2849.2044599999999</v>
+      </c>
+      <c r="I18">
+        <v>2876.2872699999998</v>
+      </c>
+      <c r="J18">
+        <v>180.49963199999999</v>
+      </c>
+      <c r="K18">
+        <v>1723.0412899999999</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>6.2035009940985422</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="1"/>
+        <v>6.2754382666373942</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="2"/>
+        <v>-7.1937272538852071E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1102,8 +1611,35 @@
       <c r="F19">
         <v>0.87858830322827552</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>182.41586000000001</v>
+      </c>
+      <c r="H19">
+        <v>2844.8296</v>
+      </c>
+      <c r="I19">
+        <v>2874.8847099999998</v>
+      </c>
+      <c r="J19">
+        <v>178.17780400000001</v>
+      </c>
+      <c r="K19">
+        <v>1727.40173</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>6.4121893276138584</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="1"/>
+        <v>6.1977373694404605</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="2"/>
+        <v>0.21445195817339791</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1122,8 +1658,35 @@
       <c r="F20">
         <v>0.87877230775366921</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>185.04153700000001</v>
+      </c>
+      <c r="H20">
+        <v>2847.51073</v>
+      </c>
+      <c r="I20">
+        <v>2873.27261</v>
+      </c>
+      <c r="J20">
+        <v>175.742302</v>
+      </c>
+      <c r="K20">
+        <v>1732.6196399999999</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>6.4983613599938925</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="1"/>
+        <v>6.1164506767772373</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="2"/>
+        <v>0.38191068321665522</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1142,8 +1705,35 @@
       <c r="F21">
         <v>0.88165781520733311</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>190.40384900000001</v>
+      </c>
+      <c r="H21">
+        <v>2843.00936</v>
+      </c>
+      <c r="I21">
+        <v>2871.3626199999999</v>
+      </c>
+      <c r="J21">
+        <v>173.305521</v>
+      </c>
+      <c r="K21">
+        <v>1738.6408699999999</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="0"/>
+        <v>6.6972642327143106</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="1"/>
+        <v>6.0356542845849264</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="2"/>
+        <v>0.66160994812938423</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1162,8 +1752,35 @@
       <c r="F22">
         <v>0.88401462271315212</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>186.62640400000001</v>
+      </c>
+      <c r="H22">
+        <v>2822.2287000000001</v>
+      </c>
+      <c r="I22">
+        <v>2866.8248699999999</v>
+      </c>
+      <c r="J22">
+        <v>170.47821099999999</v>
+      </c>
+      <c r="K22">
+        <v>1742.4371699999999</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="0"/>
+        <v>6.6127314203841809</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="1"/>
+        <v>5.9465861617141611</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="2"/>
+        <v>0.66614525867001984</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1182,8 +1799,35 @@
       <c r="F23">
         <v>0.88572913420925414</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <v>184.51916199999999</v>
+      </c>
+      <c r="H23">
+        <v>2836.2442999999998</v>
+      </c>
+      <c r="I23">
+        <v>2867.73396</v>
+      </c>
+      <c r="J23">
+        <v>167.89041499999999</v>
+      </c>
+      <c r="K23">
+        <v>1748.09374</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="0"/>
+        <v>6.5057569970259621</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="1"/>
+        <v>5.8544626991828768</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="2"/>
+        <v>0.65129429784308535</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1202,8 +1846,35 @@
       <c r="F24">
         <v>0.88712384884161277</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <v>179.896129</v>
+      </c>
+      <c r="H24">
+        <v>2826.07357</v>
+      </c>
+      <c r="I24">
+        <v>2867.3761399999999</v>
+      </c>
+      <c r="J24">
+        <v>165.13997599999999</v>
+      </c>
+      <c r="K24">
+        <v>1753.8338100000001</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="0"/>
+        <v>6.36558548615562</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="1"/>
+        <v>5.7592714710948245</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="2"/>
+        <v>0.60631401506079552</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1222,8 +1893,35 @@
       <c r="F25">
         <v>0.89190346456611114</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <v>180.13936100000001</v>
+      </c>
+      <c r="H25">
+        <v>2835.8275899999999</v>
+      </c>
+      <c r="I25">
+        <v>2867.6185099999998</v>
+      </c>
+      <c r="J25">
+        <v>162.43712099999999</v>
+      </c>
+      <c r="K25">
+        <v>1760.03342</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="0"/>
+        <v>6.3522677343018588</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="1"/>
+        <v>5.6645303562362619</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="2"/>
+        <v>0.68773737806559687</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1242,8 +1940,35 @@
       <c r="F26">
         <v>0.89346537969248296</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <v>172.979533</v>
+      </c>
+      <c r="H26">
+        <v>2841.0472399999999</v>
+      </c>
+      <c r="I26">
+        <v>2868.9706099999999</v>
+      </c>
+      <c r="J26">
+        <v>159.589966</v>
+      </c>
+      <c r="K26">
+        <v>1765.6581900000001</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="0"/>
+        <v>6.0885834830398675</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="1"/>
+        <v>5.5626211521211788</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="2"/>
+        <v>0.52596233091868871</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1262,8 +1987,35 @@
       <c r="F27">
         <v>0.89948509848488412</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <v>169.33516800000001</v>
+      </c>
+      <c r="H27">
+        <v>2852.6362899999999</v>
+      </c>
+      <c r="I27">
+        <v>2868.1002699999999</v>
+      </c>
+      <c r="J27">
+        <v>156.63649699999999</v>
+      </c>
+      <c r="K27">
+        <v>1771.4847600000001</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="0"/>
+        <v>5.9360938719601029</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="1"/>
+        <v>5.4613326681218153</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="2"/>
+        <v>0.47476120383828757</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1282,8 +2034,35 @@
       <c r="F28">
         <v>0.90625071409108326</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28">
+        <v>161.66624999999999</v>
+      </c>
+      <c r="H28">
+        <v>2849.67569</v>
+      </c>
+      <c r="I28">
+        <v>2867.06747</v>
+      </c>
+      <c r="J28">
+        <v>153.57673399999999</v>
+      </c>
+      <c r="K28">
+        <v>1776.8435099999999</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="0"/>
+        <v>5.6731455641536526</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="1"/>
+        <v>5.3565789995168824</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="2"/>
+        <v>0.31656656463677013</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1302,8 +2081,35 @@
       <c r="F29">
         <v>0.90976902476057697</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29">
+        <v>153.604668</v>
+      </c>
+      <c r="H29">
+        <v>2850.3584099999998</v>
+      </c>
+      <c r="I29">
+        <v>2865.6797799999999</v>
+      </c>
+      <c r="J29">
+        <v>150.46946399999999</v>
+      </c>
+      <c r="K29">
+        <v>1782.5222100000001</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="0"/>
+        <v>5.3889597694487836</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="1"/>
+        <v>5.2507424259384621</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="2"/>
+        <v>0.13821734351032156</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1322,8 +2128,35 @@
       <c r="F30">
         <v>0.91130623905658759</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30">
+        <v>140.58405400000001</v>
+      </c>
+      <c r="H30">
+        <v>2859.2962600000001</v>
+      </c>
+      <c r="I30">
+        <v>2863.3473300000001</v>
+      </c>
+      <c r="J30">
+        <v>147.203247</v>
+      </c>
+      <c r="K30">
+        <v>1788.3887500000001</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="0"/>
+        <v>4.9167361901840847</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="1"/>
+        <v>5.1409497359162506</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="2"/>
+        <v>-0.2242135457321659</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1342,8 +2175,35 @@
       <c r="F31">
         <v>0.91741335189723971</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31">
+        <v>132.359736</v>
+      </c>
+      <c r="H31">
+        <v>2867.7513899999999</v>
+      </c>
+      <c r="I31">
+        <v>2863.8500300000001</v>
+      </c>
+      <c r="J31">
+        <v>144.205341</v>
+      </c>
+      <c r="K31">
+        <v>1796.9067500000001</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="0"/>
+        <v>4.6154536429324162</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="1"/>
+        <v>5.0353663595994931</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="2"/>
+        <v>-0.41991271666707686</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1362,8 +2222,35 @@
       <c r="F32">
         <v>0.92238775226370417</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32">
+        <v>125.112899</v>
+      </c>
+      <c r="H32">
+        <v>2869.7239199999999</v>
+      </c>
+      <c r="I32">
+        <v>2863.6302099999998</v>
+      </c>
+      <c r="J32">
+        <v>141.23267999999999</v>
+      </c>
+      <c r="K32">
+        <v>1803.77637</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="0"/>
+        <v>4.3597538469833017</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="1"/>
+        <v>4.9319454553456463</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="2"/>
+        <v>-0.57219160836234462</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1382,8 +2269,35 @@
       <c r="F33">
         <v>0.92475014507672404</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33">
+        <v>116.22247900000001</v>
+      </c>
+      <c r="H33">
+        <v>2882.3636700000002</v>
+      </c>
+      <c r="I33">
+        <v>2864.1880900000001</v>
+      </c>
+      <c r="J33">
+        <v>138.304575</v>
+      </c>
+      <c r="K33">
+        <v>1810.0855200000001</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="0"/>
+        <v>4.0321934462905578</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="1"/>
+        <v>4.8287532331719172</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="2"/>
+        <v>-0.79655978688135942</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1402,8 +2316,35 @@
       <c r="F34">
         <v>0.92806093915285237</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <v>107.377635</v>
+      </c>
+      <c r="H34">
+        <v>2910.2888499999999</v>
+      </c>
+      <c r="I34">
+        <v>2866.68406</v>
+      </c>
+      <c r="J34">
+        <v>135.52635699999999</v>
+      </c>
+      <c r="K34">
+        <v>1817.7149899999999</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="0"/>
+        <v>3.6895868600809156</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="1"/>
+        <v>4.7276349316289847</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="2"/>
+        <v>-1.0380480715480691</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1422,8 +2363,35 @@
       <c r="F35">
         <v>0.93151863367632082</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35">
+        <v>99.576502399999995</v>
+      </c>
+      <c r="H35">
+        <v>2905.9630200000001</v>
+      </c>
+      <c r="I35">
+        <v>2867.4755</v>
+      </c>
+      <c r="J35">
+        <v>132.80515700000001</v>
+      </c>
+      <c r="K35">
+        <v>1824.2559699999999</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="0"/>
+        <v>3.4266266196326196</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="1"/>
+        <v>4.6314312711651766</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="2"/>
+        <v>-1.204804651532557</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1442,8 +2410,35 @@
       <c r="F36">
         <v>0.93187301686391322</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36">
+        <v>91.426040499999999</v>
+      </c>
+      <c r="H36">
+        <v>2891.9307899999999</v>
+      </c>
+      <c r="I36">
+        <v>2866.9708599999999</v>
+      </c>
+      <c r="J36">
+        <v>130.14165399999999</v>
+      </c>
+      <c r="K36">
+        <v>1830.6609800000001</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="0"/>
+        <v>3.1614186901063426</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="1"/>
+        <v>4.5393434518549656</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="2"/>
+        <v>-1.377924761748623</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1462,8 +2457,35 @@
       <c r="F37">
         <v>0.94588320513808066</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37">
+        <v>81.012245699999994</v>
+      </c>
+      <c r="H37">
+        <v>2886.13762</v>
+      </c>
+      <c r="I37">
+        <v>2866.7408500000001</v>
+      </c>
+      <c r="J37">
+        <v>127.595496</v>
+      </c>
+      <c r="K37">
+        <v>1837.50414</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="0"/>
+        <v>2.8069432704321282</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="1"/>
+        <v>4.4508904946884194</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="2"/>
+        <v>-1.6439472242562911</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1482,8 +2504,35 @@
       <c r="F38">
         <v>0.95760039033652811</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38">
+        <v>70.6699141</v>
+      </c>
+      <c r="H38">
+        <v>2907.96992</v>
+      </c>
+      <c r="I38">
+        <v>2869.92308</v>
+      </c>
+      <c r="J38">
+        <v>125.399975</v>
+      </c>
+      <c r="K38">
+        <v>1844.48262</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="0"/>
+        <v>2.4302147561416314</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="1"/>
+        <v>4.3694542154767442</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="2"/>
+        <v>-1.9392394593351128</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1502,8 +2551,35 @@
       <c r="F39">
         <v>0.96601538163254197</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39">
+        <v>61.9161158</v>
+      </c>
+      <c r="H39">
+        <v>2898.1729099999998</v>
+      </c>
+      <c r="I39">
+        <v>2871.40263</v>
+      </c>
+      <c r="J39">
+        <v>123.446561</v>
+      </c>
+      <c r="K39">
+        <v>1850.1093699999999</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="0"/>
+        <v>2.1363844643762131</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="1"/>
+        <v>4.2991728053129208</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="2"/>
+        <v>-2.1627883409367077</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1522,8 +2598,35 @@
       <c r="F40">
         <v>0.97427767078015248</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40">
+        <v>63.451785100000002</v>
+      </c>
+      <c r="H40">
+        <v>2911.3177900000001</v>
+      </c>
+      <c r="I40">
+        <v>2874.49377</v>
+      </c>
+      <c r="J40">
+        <v>122.067229</v>
+      </c>
+      <c r="K40">
+        <v>1855.9829199999999</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="0"/>
+        <v>2.1794867368292352</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="1"/>
+        <v>4.2465643959284005</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="2"/>
+        <v>-2.0670776590991653</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1542,8 +2645,35 @@
       <c r="F41">
         <v>0.97453486577621307</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41">
+        <v>73.022736699999996</v>
+      </c>
+      <c r="H41">
+        <v>2914.9343399999998</v>
+      </c>
+      <c r="I41">
+        <v>2877.2009600000001</v>
+      </c>
+      <c r="J41">
+        <v>121.147987</v>
+      </c>
+      <c r="K41">
+        <v>1860.64184</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="0"/>
+        <v>2.5051245819828658</v>
+      </c>
+      <c r="M41">
+        <f t="shared" si="1"/>
+        <v>4.2106195807747815</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="2"/>
+        <v>-1.7054949987919157</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1562,8 +2692,35 @@
       <c r="F42">
         <v>0.97309986997876508</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42">
+        <v>93.462480200000002</v>
+      </c>
+      <c r="H42">
+        <v>2884.3014400000002</v>
+      </c>
+      <c r="I42">
+        <v>2876.9850499999998</v>
+      </c>
+      <c r="J42">
+        <v>120.621922</v>
+      </c>
+      <c r="K42">
+        <v>1864.26394</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="0"/>
+        <v>3.240385311460372</v>
+      </c>
+      <c r="M42">
+        <f t="shared" si="1"/>
+        <v>4.1926502885373012</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="2"/>
+        <v>-0.95226497707692914</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1582,8 +2739,35 @@
       <c r="F43">
         <v>0.9763593901953298</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43">
+        <v>120.49818</v>
+      </c>
+      <c r="H43">
+        <v>2875.19607</v>
+      </c>
+      <c r="I43">
+        <v>2877.39797</v>
+      </c>
+      <c r="J43">
+        <v>120.454617</v>
+      </c>
+      <c r="K43">
+        <v>1866.88283</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="0"/>
+        <v>4.1909552276203552</v>
+      </c>
+      <c r="M43">
+        <f t="shared" si="1"/>
+        <v>4.1862341690607368</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="2"/>
+        <v>4.7210585596184629E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -1602,8 +2786,35 @@
       <c r="F44">
         <v>0.98041360197630611</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44">
+        <v>134.50752800000001</v>
+      </c>
+      <c r="H44">
+        <v>2870.6467600000001</v>
+      </c>
+      <c r="I44">
+        <v>2875.9954200000002</v>
+      </c>
+      <c r="J44">
+        <v>120.076724</v>
+      </c>
+      <c r="K44">
+        <v>1869.6542199999999</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="0"/>
+        <v>4.6856175365860757</v>
+      </c>
+      <c r="M44">
+        <f t="shared" si="1"/>
+        <v>4.1751361342571256</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="2"/>
+        <v>0.51048140232895012</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -1622,8 +2833,35 @@
       <c r="F45">
         <v>0.98420761482177277</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45">
+        <v>144.740711</v>
+      </c>
+      <c r="H45">
+        <v>2857.07573</v>
+      </c>
+      <c r="I45">
+        <v>2873.9134100000001</v>
+      </c>
+      <c r="J45">
+        <v>119.69146000000001</v>
+      </c>
+      <c r="K45">
+        <v>1871.43235</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="0"/>
+        <v>5.0660439091686245</v>
+      </c>
+      <c r="M45">
+        <f t="shared" si="1"/>
+        <v>4.1647552631030731</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="2"/>
+        <v>0.90128864606555137</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -1642,8 +2880,35 @@
       <c r="F46">
         <v>0.99155302954466507</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46">
+        <v>149.454419</v>
+      </c>
+      <c r="H46">
+        <v>2829.8395799999998</v>
+      </c>
+      <c r="I46">
+        <v>2869.9863599999999</v>
+      </c>
+      <c r="J46">
+        <v>119.191529</v>
+      </c>
+      <c r="K46">
+        <v>1872.4585400000001</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="0"/>
+        <v>5.2813742537306663</v>
+      </c>
+      <c r="M46">
+        <f t="shared" si="1"/>
+        <v>4.153034685502826</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="2"/>
+        <v>1.1283395682278403</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -1662,8 +2927,35 @@
       <c r="F47">
         <v>0.99637985019310416</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G47">
+        <v>147.40721500000001</v>
+      </c>
+      <c r="H47">
+        <v>2832.2677399999998</v>
+      </c>
+      <c r="I47">
+        <v>2869.3366500000002</v>
+      </c>
+      <c r="J47">
+        <v>118.701325</v>
+      </c>
+      <c r="K47">
+        <v>1874.8527300000001</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="0"/>
+        <v>5.2045649822640012</v>
+      </c>
+      <c r="M47">
+        <f t="shared" si="1"/>
+        <v>4.136890838514887</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="2"/>
+        <v>1.0676741437491142</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -1682,8 +2974,35 @@
       <c r="F48">
         <v>1.0034412821308867</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48">
+        <v>147.05524</v>
+      </c>
+      <c r="H48">
+        <v>2833.35581</v>
+      </c>
+      <c r="I48">
+        <v>2868.2967199999998</v>
+      </c>
+      <c r="J48">
+        <v>118.271389</v>
+      </c>
+      <c r="K48">
+        <v>1877.4094600000001</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="0"/>
+        <v>5.1901437680712608</v>
+      </c>
+      <c r="M48">
+        <f t="shared" si="1"/>
+        <v>4.1234014659403861</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="2"/>
+        <v>1.0667423021308746</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -1702,8 +3021,35 @@
       <c r="F49">
         <v>1.0086263117726171</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49">
+        <v>145.60143600000001</v>
+      </c>
+      <c r="H49">
+        <v>2832.78611</v>
+      </c>
+      <c r="I49">
+        <v>2867.5267699999999</v>
+      </c>
+      <c r="J49">
+        <v>117.86864300000001</v>
+      </c>
+      <c r="K49">
+        <v>1879.56378</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="0"/>
+        <v>5.1398669135665873</v>
+      </c>
+      <c r="M49">
+        <f t="shared" si="1"/>
+        <v>4.1104635616008567</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="2"/>
+        <v>1.0294033519657306</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -1722,8 +3068,35 @@
       <c r="F50">
         <v>1.016896339700625</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G50">
+        <v>142.71013199999999</v>
+      </c>
+      <c r="H50">
+        <v>2823.5940599999999</v>
+      </c>
+      <c r="I50">
+        <v>2865.8201199999999</v>
+      </c>
+      <c r="J50">
+        <v>117.446302</v>
+      </c>
+      <c r="K50">
+        <v>1881.12897</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="0"/>
+        <v>5.0542014527399877</v>
+      </c>
+      <c r="M50">
+        <f t="shared" si="1"/>
+        <v>4.0981742427015977</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="2"/>
+        <v>0.95602721003838997</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -1742,8 +3115,35 @@
       <c r="F51">
         <v>1.0259983724379484</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G51">
+        <v>140.69333399999999</v>
+      </c>
+      <c r="H51">
+        <v>2831.3271399999999</v>
+      </c>
+      <c r="I51">
+        <v>2865.8269100000002</v>
+      </c>
+      <c r="J51">
+        <v>117.140137</v>
+      </c>
+      <c r="K51">
+        <v>1883.78388</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="0"/>
+        <v>4.9691655906636063</v>
+      </c>
+      <c r="M51">
+        <f t="shared" si="1"/>
+        <v>4.087481228934374</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="2"/>
+        <v>0.88168436172923226</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -1762,8 +3162,35 @@
       <c r="F52">
         <v>1.0289114015916663</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G52">
+        <v>141.11979099999999</v>
+      </c>
+      <c r="H52">
+        <v>2832.87635</v>
+      </c>
+      <c r="I52">
+        <v>2865.5961499999999</v>
+      </c>
+      <c r="J52">
+        <v>116.934679</v>
+      </c>
+      <c r="K52">
+        <v>1885.73215</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="0"/>
+        <v>4.9815019635431668</v>
+      </c>
+      <c r="M52">
+        <f t="shared" si="1"/>
+        <v>4.080640567583119</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="2"/>
+        <v>0.90086139596004777</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -1782,8 +3209,35 @@
       <c r="F53">
         <v>1.0342054267044236</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G53">
+        <v>139.15328</v>
+      </c>
+      <c r="H53">
+        <v>2831.4003600000001</v>
+      </c>
+      <c r="I53">
+        <v>2865.4603400000001</v>
+      </c>
+      <c r="J53">
+        <v>120.10899999999999</v>
+      </c>
+      <c r="K53">
+        <v>1887.1251</v>
+      </c>
+      <c r="L53">
+        <f t="shared" si="0"/>
+        <v>4.9146451334067072</v>
+      </c>
+      <c r="M53">
+        <f t="shared" si="1"/>
+        <v>4.1916127165801216</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="2"/>
+        <v>0.72303241682658559</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -1802,8 +3256,35 @@
       <c r="F54">
         <v>1.0446634475409882</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G54">
+        <v>142.745969</v>
+      </c>
+      <c r="H54">
+        <v>2822.47318</v>
+      </c>
+      <c r="I54">
+        <v>2863.6863400000002</v>
+      </c>
+      <c r="J54">
+        <v>119.7663</v>
+      </c>
+      <c r="K54">
+        <v>1889.20399</v>
+      </c>
+      <c r="L54">
+        <f t="shared" si="0"/>
+        <v>5.0574783141074882</v>
+      </c>
+      <c r="M54">
+        <f t="shared" si="1"/>
+        <v>4.1822422493379632</v>
+      </c>
+      <c r="N54">
+        <f t="shared" si="2"/>
+        <v>0.87523606476952498</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -1822,8 +3303,35 @@
       <c r="F55">
         <v>1.0481304864327634</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G55">
+        <v>148.979814</v>
+      </c>
+      <c r="H55">
+        <v>2823.90229</v>
+      </c>
+      <c r="I55">
+        <v>2863.90371</v>
+      </c>
+      <c r="J55">
+        <v>120.0206</v>
+      </c>
+      <c r="K55">
+        <v>1891.9025099999999</v>
+      </c>
+      <c r="L55">
+        <f t="shared" si="0"/>
+        <v>5.2756717017995687</v>
+      </c>
+      <c r="M55">
+        <f t="shared" si="1"/>
+        <v>4.1908043060567843</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="2"/>
+        <v>1.0848673957427843</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -1842,8 +3350,35 @@
       <c r="F56">
         <v>1.0540705196882487</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G56">
+        <v>149.20548199999999</v>
+      </c>
+      <c r="H56">
+        <v>2821.3447099999998</v>
+      </c>
+      <c r="I56">
+        <v>2863.6912600000001</v>
+      </c>
+      <c r="J56">
+        <v>120.2223</v>
+      </c>
+      <c r="K56">
+        <v>1894.5120400000001</v>
+      </c>
+      <c r="L56">
+        <f t="shared" si="0"/>
+        <v>5.28845275343898</v>
+      </c>
+      <c r="M56">
+        <f t="shared" si="1"/>
+        <v>4.1981585682529206</v>
+      </c>
+      <c r="N56">
+        <f t="shared" si="2"/>
+        <v>1.0902941851860595</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -1862,8 +3397,35 @@
       <c r="F57">
         <v>1.0557085352741276</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G57">
+        <v>147.44329099999999</v>
+      </c>
+      <c r="H57">
+        <v>2820.65924</v>
+      </c>
+      <c r="I57">
+        <v>2862.8768500000001</v>
+      </c>
+      <c r="J57">
+        <v>120.2491</v>
+      </c>
+      <c r="K57">
+        <v>1897.1340700000001</v>
+      </c>
+      <c r="L57">
+        <f t="shared" si="0"/>
+        <v>5.2272635031234751</v>
+      </c>
+      <c r="M57">
+        <f t="shared" si="1"/>
+        <v>4.2002889506057519</v>
+      </c>
+      <c r="N57">
+        <f t="shared" si="2"/>
+        <v>1.0269745525177232</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -1882,8 +3444,35 @@
       <c r="F58">
         <v>1.054525544330823</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G58">
+        <v>145.69206</v>
+      </c>
+      <c r="H58">
+        <v>2818.7222499999998</v>
+      </c>
+      <c r="I58">
+        <v>2863.26199</v>
+      </c>
+      <c r="J58">
+        <v>119.416</v>
+      </c>
+      <c r="K58">
+        <v>1900.5233499999999</v>
+      </c>
+      <c r="L58">
+        <f t="shared" si="0"/>
+        <v>5.1687270712820323</v>
+      </c>
+      <c r="M58">
+        <f t="shared" si="1"/>
+        <v>4.1706277810784611</v>
+      </c>
+      <c r="N58">
+        <f t="shared" si="2"/>
+        <v>0.99809929020357124</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -1902,8 +3491,35 @@
       <c r="F59">
         <v>1.0547765527205404</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G59">
+        <v>145.77926500000001</v>
+      </c>
+      <c r="H59">
+        <v>2820.61384</v>
+      </c>
+      <c r="I59">
+        <v>2863.2533600000002</v>
+      </c>
+      <c r="J59">
+        <v>119.22410000000001</v>
+      </c>
+      <c r="K59">
+        <v>1903.3150000000001</v>
+      </c>
+      <c r="L59">
+        <f t="shared" si="0"/>
+        <v>5.1683524675607497</v>
+      </c>
+      <c r="M59">
+        <f t="shared" si="1"/>
+        <v>4.1639381853375355</v>
+      </c>
+      <c r="N59">
+        <f t="shared" si="2"/>
+        <v>1.0044142822232143</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -1922,8 +3538,35 @@
       <c r="F60">
         <v>1.0560285660651176</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G60">
+        <v>141.94360499999999</v>
+      </c>
+      <c r="H60">
+        <v>2824.6955800000001</v>
+      </c>
+      <c r="I60">
+        <v>2864.0382</v>
+      </c>
+      <c r="J60">
+        <v>118.01430000000001</v>
+      </c>
+      <c r="K60">
+        <v>1907.49899</v>
+      </c>
+      <c r="L60">
+        <f t="shared" si="0"/>
+        <v>5.0250938899405222</v>
+      </c>
+      <c r="M60">
+        <f t="shared" si="1"/>
+        <v>4.1205560735886833</v>
+      </c>
+      <c r="N60">
+        <f t="shared" si="2"/>
+        <v>0.90453781635183894</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -1942,8 +3585,35 @@
       <c r="F61">
         <v>1.0591075723279042</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G61">
+        <v>139.174914</v>
+      </c>
+      <c r="H61">
+        <v>2826.7089099999998</v>
+      </c>
+      <c r="I61">
+        <v>2865.3390199999999</v>
+      </c>
+      <c r="J61">
+        <v>116.51090000000001</v>
+      </c>
+      <c r="K61">
+        <v>1911.77874</v>
+      </c>
+      <c r="L61">
+        <f t="shared" si="0"/>
+        <v>4.9235672448494183</v>
+      </c>
+      <c r="M61">
+        <f t="shared" si="1"/>
+        <v>4.0662169183735895</v>
+      </c>
+      <c r="N61">
+        <f t="shared" si="2"/>
+        <v>0.85735032647582887</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -1962,8 +3632,35 @@
       <c r="F62">
         <v>1.0596095721924428</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G62">
+        <v>130.459924</v>
+      </c>
+      <c r="H62">
+        <v>2822.3292499999998</v>
+      </c>
+      <c r="I62">
+        <v>2868.98875</v>
+      </c>
+      <c r="J62">
+        <v>116.5296</v>
+      </c>
+      <c r="K62">
+        <v>1916.6791800000001</v>
+      </c>
+      <c r="L62">
+        <f t="shared" si="0"/>
+        <v>4.622420435177788</v>
+      </c>
+      <c r="M62">
+        <f t="shared" si="1"/>
+        <v>4.0616959547157512</v>
+      </c>
+      <c r="N62">
+        <f t="shared" si="2"/>
+        <v>0.56072448046203682</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -1982,8 +3679,35 @@
       <c r="F63">
         <v>1.059295563489151</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G63">
+        <v>126.989583</v>
+      </c>
+      <c r="H63">
+        <v>2825.7004499999998</v>
+      </c>
+      <c r="I63">
+        <v>2872.6384699999999</v>
+      </c>
+      <c r="J63">
+        <v>115.599041</v>
+      </c>
+      <c r="K63">
+        <v>1921.8831600000001</v>
+      </c>
+      <c r="L63">
+        <f t="shared" si="0"/>
+        <v>4.4940921816394228</v>
+      </c>
+      <c r="M63">
+        <f t="shared" si="1"/>
+        <v>4.0241416456418895</v>
+      </c>
+      <c r="N63">
+        <f t="shared" si="2"/>
+        <v>0.46995053599753334</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -2002,8 +3726,35 @@
       <c r="F64">
         <v>1.0595845521370582</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G64">
+        <v>125.009658</v>
+      </c>
+      <c r="H64">
+        <v>2827.5064200000002</v>
+      </c>
+      <c r="I64">
+        <v>2876.2882</v>
+      </c>
+      <c r="J64">
+        <v>115.054439</v>
+      </c>
+      <c r="K64">
+        <v>1927.68174</v>
+      </c>
+      <c r="L64">
+        <f t="shared" si="0"/>
+        <v>4.4211980250782243</v>
+      </c>
+      <c r="M64">
+        <f t="shared" si="1"/>
+        <v>4.0001012068262147</v>
+      </c>
+      <c r="N64">
+        <f t="shared" si="2"/>
+        <v>0.42109681825200962</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -2022,8 +3773,35 @@
       <c r="F65">
         <v>1.0608635445243091</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G65">
+        <v>123.36059899999999</v>
+      </c>
+      <c r="H65">
+        <v>2833.9921599999998</v>
+      </c>
+      <c r="I65">
+        <v>2879.9379199999998</v>
+      </c>
+      <c r="J65">
+        <v>113.826075</v>
+      </c>
+      <c r="K65">
+        <v>1933.8398999999999</v>
+      </c>
+      <c r="L65">
+        <f t="shared" si="0"/>
+        <v>4.3528913290995135</v>
+      </c>
+      <c r="M65">
+        <f t="shared" si="1"/>
+        <v>3.9523794665685021</v>
+      </c>
+      <c r="N65">
+        <f t="shared" si="2"/>
+        <v>0.40051186253101134</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -2042,8 +3820,35 @@
       <c r="F66">
         <v>1.0597515370996338</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G66">
+        <v>122.25613</v>
+      </c>
+      <c r="H66">
+        <v>2845.0744</v>
+      </c>
+      <c r="I66">
+        <v>2885.72282</v>
+      </c>
+      <c r="J66">
+        <v>113.46207099999999</v>
+      </c>
+      <c r="K66">
+        <v>1940.45363</v>
+      </c>
+      <c r="L66">
+        <f t="shared" si="0"/>
+        <v>4.2971153935376876</v>
+      </c>
+      <c r="M66">
+        <f t="shared" si="1"/>
+        <v>3.9318423174128689</v>
+      </c>
+      <c r="N66">
+        <f t="shared" si="2"/>
+        <v>0.36527307612481863</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -2062,8 +3867,35 @@
       <c r="F67">
         <v>1.0638215426616002</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G67">
+        <v>121.365228</v>
+      </c>
+      <c r="H67">
+        <v>2853.6372000000001</v>
+      </c>
+      <c r="I67">
+        <v>2891.5077200000001</v>
+      </c>
+      <c r="J67">
+        <v>112.964885</v>
+      </c>
+      <c r="K67">
+        <v>1947.43595</v>
+      </c>
+      <c r="L67">
+        <f t="shared" ref="L67:L97" si="3">G67/H67*100</f>
+        <v>4.2530013275689003</v>
+      </c>
+      <c r="M67">
+        <f t="shared" ref="M67:M97" si="4">J67/I67*100</f>
+        <v>3.906781372867993</v>
+      </c>
+      <c r="N67">
+        <f t="shared" ref="N67:N97" si="5">L67-M67</f>
+        <v>0.34621995470090727</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -2082,8 +3914,35 @@
       <c r="F68">
         <v>1.0629575523522772</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G68">
+        <v>116.519723</v>
+      </c>
+      <c r="H68">
+        <v>2858.2902300000001</v>
+      </c>
+      <c r="I68">
+        <v>2897.2926200000002</v>
+      </c>
+      <c r="J68">
+        <v>111.796069</v>
+      </c>
+      <c r="K68">
+        <v>1954.6157499999999</v>
+      </c>
+      <c r="L68">
+        <f t="shared" si="3"/>
+        <v>4.0765532407113181</v>
+      </c>
+      <c r="M68">
+        <f t="shared" si="4"/>
+        <v>3.8586392077994525</v>
+      </c>
+      <c r="N68">
+        <f t="shared" si="5"/>
+        <v>0.21791403291186562</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -2102,8 +3961,35 @@
       <c r="F69">
         <v>1.0624845641454703</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G69">
+        <v>113.395698</v>
+      </c>
+      <c r="H69">
+        <v>2865.5751300000002</v>
+      </c>
+      <c r="I69">
+        <v>2902.8225200000002</v>
+      </c>
+      <c r="J69">
+        <v>111.832125</v>
+      </c>
+      <c r="K69">
+        <v>1961.71046</v>
+      </c>
+      <c r="L69">
+        <f t="shared" si="3"/>
+        <v>3.9571706500677228</v>
+      </c>
+      <c r="M69">
+        <f t="shared" si="4"/>
+        <v>3.8525305708321431</v>
+      </c>
+      <c r="N69">
+        <f t="shared" si="5"/>
+        <v>0.10464007923557972</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -2122,8 +4008,35 @@
       <c r="F70">
         <v>1.0608735743350028</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G70">
+        <v>110.98995499999999</v>
+      </c>
+      <c r="H70">
+        <v>2876.30951</v>
+      </c>
+      <c r="I70">
+        <v>2908.6488399999998</v>
+      </c>
+      <c r="J70">
+        <v>111.82916</v>
+      </c>
+      <c r="K70">
+        <v>1969.31062</v>
+      </c>
+      <c r="L70">
+        <f t="shared" si="3"/>
+        <v>3.8587625780231138</v>
+      </c>
+      <c r="M70">
+        <f t="shared" si="4"/>
+        <v>3.8447116221839965</v>
+      </c>
+      <c r="N70">
+        <f t="shared" si="5"/>
+        <v>1.4050955839117307E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -2142,8 +4055,35 @@
       <c r="F71">
         <v>1.0630395945153628</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G71">
+        <v>108.271762</v>
+      </c>
+      <c r="H71">
+        <v>2884.0498400000001</v>
+      </c>
+      <c r="I71">
+        <v>2915.0189599999999</v>
+      </c>
+      <c r="J71">
+        <v>112.356604</v>
+      </c>
+      <c r="K71">
+        <v>1977.65751</v>
+      </c>
+      <c r="L71">
+        <f t="shared" si="3"/>
+        <v>3.7541571056899627</v>
+      </c>
+      <c r="M71">
+        <f t="shared" si="4"/>
+        <v>3.8544038835342604</v>
+      </c>
+      <c r="N71">
+        <f t="shared" si="5"/>
+        <v>-0.1002467778442977</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -2162,8 +4102,35 @@
       <c r="F72">
         <v>1.0617066079712385</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G72">
+        <v>107.28928000000001</v>
+      </c>
+      <c r="H72">
+        <v>2896.1749799999998</v>
+      </c>
+      <c r="I72">
+        <v>2925.9920900000002</v>
+      </c>
+      <c r="J72">
+        <v>117.470153</v>
+      </c>
+      <c r="K72">
+        <v>1985.71703</v>
+      </c>
+      <c r="L72">
+        <f t="shared" si="3"/>
+        <v>3.7045164998973932</v>
+      </c>
+      <c r="M72">
+        <f t="shared" si="4"/>
+        <v>4.0147119126354163</v>
+      </c>
+      <c r="N72">
+        <f t="shared" si="5"/>
+        <v>-0.31019541273802309</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -2182,8 +4149,35 @@
       <c r="F73">
         <v>1.0642906255739908</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G73">
+        <v>109.172597</v>
+      </c>
+      <c r="H73">
+        <v>2909.7444700000001</v>
+      </c>
+      <c r="I73">
+        <v>2936.5749700000001</v>
+      </c>
+      <c r="J73">
+        <v>122.177819</v>
+      </c>
+      <c r="K73">
+        <v>1998.2604100000001</v>
+      </c>
+      <c r="L73">
+        <f t="shared" si="3"/>
+        <v>3.7519650995332929</v>
+      </c>
+      <c r="M73">
+        <f t="shared" si="4"/>
+        <v>4.1605550768554016</v>
+      </c>
+      <c r="N73">
+        <f t="shared" si="5"/>
+        <v>-0.40858997732210867</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -2202,8 +4196,35 @@
       <c r="F74">
         <v>1.0698616520696393</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G74">
+        <v>112.34479899999999</v>
+      </c>
+      <c r="H74">
+        <v>2921.6062000000002</v>
+      </c>
+      <c r="I74">
+        <v>2949.3186500000002</v>
+      </c>
+      <c r="J74">
+        <v>126.079179</v>
+      </c>
+      <c r="K74">
+        <v>2007.52189</v>
+      </c>
+      <c r="L74">
+        <f t="shared" si="3"/>
+        <v>3.8453094397184668</v>
+      </c>
+      <c r="M74">
+        <f t="shared" si="4"/>
+        <v>4.2748578218226774</v>
+      </c>
+      <c r="N74">
+        <f t="shared" si="5"/>
+        <v>-0.42954838210421054</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -2222,8 +4243,35 @@
       <c r="F75">
         <v>1.0708516805761383</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G75">
+        <v>112.63160999999999</v>
+      </c>
+      <c r="H75">
+        <v>2933.3497299999999</v>
+      </c>
+      <c r="I75">
+        <v>2958.6159299999999</v>
+      </c>
+      <c r="J75">
+        <v>128.62748199999999</v>
+      </c>
+      <c r="K75">
+        <v>2016.5584899999999</v>
+      </c>
+      <c r="L75">
+        <f t="shared" si="3"/>
+        <v>3.8396925142642298</v>
+      </c>
+      <c r="M75">
+        <f t="shared" si="4"/>
+        <v>4.3475559195005076</v>
+      </c>
+      <c r="N75">
+        <f t="shared" si="5"/>
+        <v>-0.50786340523627782</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -2242,8 +4290,35 @@
       <c r="F76">
         <v>1.0774707287977836</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G76">
+        <v>114.665547</v>
+      </c>
+      <c r="H76">
+        <v>2942.2687799999999</v>
+      </c>
+      <c r="I76">
+        <v>2967.0917800000002</v>
+      </c>
+      <c r="J76">
+        <v>128.059157</v>
+      </c>
+      <c r="K76">
+        <v>2027.18523</v>
+      </c>
+      <c r="L76">
+        <f t="shared" si="3"/>
+        <v>3.8971812425647943</v>
+      </c>
+      <c r="M76">
+        <f t="shared" si="4"/>
+        <v>4.315982332032883</v>
+      </c>
+      <c r="N76">
+        <f t="shared" si="5"/>
+        <v>-0.41880108946808869</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -2262,8 +4337,35 @@
       <c r="F77">
         <v>1.0768027680057819</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G77">
+        <v>111.76178299999999</v>
+      </c>
+      <c r="H77">
+        <v>2950.5178900000001</v>
+      </c>
+      <c r="I77">
+        <v>2974.6704500000001</v>
+      </c>
+      <c r="J77">
+        <v>126.476236</v>
+      </c>
+      <c r="K77">
+        <v>2037.83086</v>
+      </c>
+      <c r="L77">
+        <f t="shared" si="3"/>
+        <v>3.7878700338942868</v>
+      </c>
+      <c r="M77">
+        <f t="shared" si="4"/>
+        <v>4.2517730325387815</v>
+      </c>
+      <c r="N77">
+        <f t="shared" si="5"/>
+        <v>-0.46390299864449469</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -2282,8 +4384,35 @@
       <c r="F78">
         <v>1.0750528124297811</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G78">
+        <v>108.389957</v>
+      </c>
+      <c r="H78">
+        <v>2956.7958100000001</v>
+      </c>
+      <c r="I78">
+        <v>2980.94218</v>
+      </c>
+      <c r="J78">
+        <v>125.22589000000001</v>
+      </c>
+      <c r="K78">
+        <v>2047.9069199999999</v>
+      </c>
+      <c r="L78">
+        <f t="shared" si="3"/>
+        <v>3.6657910780792129</v>
+      </c>
+      <c r="M78">
+        <f t="shared" si="4"/>
+        <v>4.2008828899861452</v>
+      </c>
+      <c r="N78">
+        <f t="shared" si="5"/>
+        <v>-0.53509181190693234</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -2302,8 +4431,35 @@
       <c r="F79">
         <v>1.0812008587515869</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G79">
+        <v>105.629001</v>
+      </c>
+      <c r="H79">
+        <v>2965.7101699999998</v>
+      </c>
+      <c r="I79">
+        <v>2987.4463500000002</v>
+      </c>
+      <c r="J79">
+        <v>124.179086</v>
+      </c>
+      <c r="K79">
+        <v>2059.49325</v>
+      </c>
+      <c r="L79">
+        <f t="shared" si="3"/>
+        <v>3.5616764601107334</v>
+      </c>
+      <c r="M79">
+        <f t="shared" si="4"/>
+        <v>4.156696772144544</v>
+      </c>
+      <c r="N79">
+        <f t="shared" si="5"/>
+        <v>-0.59502031203381067</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -2322,8 +4478,35 @@
       <c r="F80">
         <v>1.0849219029477879</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G80">
+        <v>103.41573699999999</v>
+      </c>
+      <c r="H80">
+        <v>2977.1850300000001</v>
+      </c>
+      <c r="I80">
+        <v>2993.6262099999999</v>
+      </c>
+      <c r="J80">
+        <v>122.840339</v>
+      </c>
+      <c r="K80">
+        <v>2068.0679</v>
+      </c>
+      <c r="L80">
+        <f t="shared" si="3"/>
+        <v>3.4736079873409813</v>
+      </c>
+      <c r="M80">
+        <f t="shared" si="4"/>
+        <v>4.1033960281901729</v>
+      </c>
+      <c r="N80">
+        <f t="shared" si="5"/>
+        <v>-0.6297880408491916</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -2342,8 +4525,35 @@
       <c r="F81">
         <v>1.0842999414808316</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G81">
+        <v>103.164136</v>
+      </c>
+      <c r="H81">
+        <v>2982.19497</v>
+      </c>
+      <c r="I81">
+        <v>2999.6252500000001</v>
+      </c>
+      <c r="J81">
+        <v>121.33444799999999</v>
+      </c>
+      <c r="K81">
+        <v>2079.4666999999999</v>
+      </c>
+      <c r="L81">
+        <f t="shared" si="3"/>
+        <v>3.459335725457279</v>
+      </c>
+      <c r="M81">
+        <f t="shared" si="4"/>
+        <v>4.0449868862785436</v>
+      </c>
+      <c r="N81">
+        <f t="shared" si="5"/>
+        <v>-0.58565116082126467</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -2362,8 +4572,35 @@
       <c r="F82">
         <v>1.0872289860620039</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G82">
+        <v>101.19964</v>
+      </c>
+      <c r="H82">
+        <v>2991.3098</v>
+      </c>
+      <c r="I82">
+        <v>3003.6910200000002</v>
+      </c>
+      <c r="J82">
+        <v>120.09346600000001</v>
+      </c>
+      <c r="K82">
+        <v>2088.9252799999999</v>
+      </c>
+      <c r="L82">
+        <f t="shared" si="3"/>
+        <v>3.3831213336712898</v>
+      </c>
+      <c r="M82">
+        <f t="shared" si="4"/>
+        <v>3.9981963923839277</v>
+      </c>
+      <c r="N82">
+        <f t="shared" si="5"/>
+        <v>-0.6150750587126379</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -2382,8 +4619,35 @@
       <c r="F83">
         <v>1.0890270289156458</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G83">
+        <v>99.902438500000002</v>
+      </c>
+      <c r="H83">
+        <v>2997.7643200000002</v>
+      </c>
+      <c r="I83">
+        <v>3007.9255199999998</v>
+      </c>
+      <c r="J83">
+        <v>118.91608100000001</v>
+      </c>
+      <c r="K83">
+        <v>2097.8122899999998</v>
+      </c>
+      <c r="L83">
+        <f t="shared" si="3"/>
+        <v>3.3325647994903078</v>
+      </c>
+      <c r="M83">
+        <f t="shared" si="4"/>
+        <v>3.9534250502319623</v>
+      </c>
+      <c r="N83">
+        <f t="shared" si="5"/>
+        <v>-0.62086025074165452</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -2402,8 +4666,35 @@
       <c r="F84">
         <v>1.0893600663969343</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G84">
+        <v>102.227957</v>
+      </c>
+      <c r="H84">
+        <v>3009.72894</v>
+      </c>
+      <c r="I84">
+        <v>3012.3111100000001</v>
+      </c>
+      <c r="J84">
+        <v>117.975556</v>
+      </c>
+      <c r="K84">
+        <v>2105.8855400000002</v>
+      </c>
+      <c r="L84">
+        <f t="shared" si="3"/>
+        <v>3.3965835142615872</v>
+      </c>
+      <c r="M84">
+        <f t="shared" si="4"/>
+        <v>3.9164465983727683</v>
+      </c>
+      <c r="N84">
+        <f t="shared" si="5"/>
+        <v>-0.5198630841111811</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -2422,8 +4713,35 @@
       <c r="F85">
         <v>1.0914081048259294</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G85">
+        <v>104.065271</v>
+      </c>
+      <c r="H85">
+        <v>3015.1360800000002</v>
+      </c>
+      <c r="I85">
+        <v>3016.83185</v>
+      </c>
+      <c r="J85">
+        <v>117.06971900000001</v>
+      </c>
+      <c r="K85">
+        <v>2113.5398599999999</v>
+      </c>
+      <c r="L85">
+        <f t="shared" si="3"/>
+        <v>3.4514286665297038</v>
+      </c>
+      <c r="M85">
+        <f t="shared" si="4"/>
+        <v>3.8805516787420551</v>
+      </c>
+      <c r="N85">
+        <f t="shared" si="5"/>
+        <v>-0.42912301221235127</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -2442,8 +4760,35 @@
       <c r="F86">
         <v>1.0933501478098677</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G86">
+        <v>106.172878</v>
+      </c>
+      <c r="H86">
+        <v>3019.2933499999999</v>
+      </c>
+      <c r="I86">
+        <v>3021.0710899999999</v>
+      </c>
+      <c r="J86">
+        <v>116.112403</v>
+      </c>
+      <c r="K86">
+        <v>2118.0178000000001</v>
+      </c>
+      <c r="L86">
+        <f t="shared" si="3"/>
+        <v>3.5164810335504497</v>
+      </c>
+      <c r="M86">
+        <f t="shared" si="4"/>
+        <v>3.8434184281310637</v>
+      </c>
+      <c r="N86">
+        <f t="shared" si="5"/>
+        <v>-0.32693739458061399</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -2462,8 +4807,35 @@
       <c r="F87">
         <v>1.0889491902483661</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G87">
+        <v>149.43236400000001</v>
+      </c>
+      <c r="H87">
+        <v>2990.16824</v>
+      </c>
+      <c r="I87">
+        <v>3025.64237</v>
+      </c>
+      <c r="J87">
+        <v>116.333547</v>
+      </c>
+      <c r="K87">
+        <v>2122.3657800000001</v>
+      </c>
+      <c r="L87">
+        <f t="shared" si="3"/>
+        <v>4.9974567317322593</v>
+      </c>
+      <c r="M87">
+        <f t="shared" si="4"/>
+        <v>3.8449206077187501</v>
+      </c>
+      <c r="N87">
+        <f t="shared" si="5"/>
+        <v>1.1525361240135092</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -2482,8 +4854,35 @@
       <c r="F88">
         <v>1.0939532247984849</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G88">
+        <v>137.55449100000001</v>
+      </c>
+      <c r="H88">
+        <v>3022.3491899999999</v>
+      </c>
+      <c r="I88">
+        <v>3029.6244099999999</v>
+      </c>
+      <c r="J88">
+        <v>114.8075</v>
+      </c>
+      <c r="K88">
+        <v>2131.09256</v>
+      </c>
+      <c r="L88">
+        <f t="shared" si="3"/>
+        <v>4.5512441598450772</v>
+      </c>
+      <c r="M88">
+        <f t="shared" si="4"/>
+        <v>3.7894961375756804</v>
+      </c>
+      <c r="N88">
+        <f t="shared" si="5"/>
+        <v>0.76174802226939686</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -2502,8 +4901,35 @@
       <c r="F89">
         <v>1.0952732697290883</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G89">
+        <v>129.15142900000001</v>
+      </c>
+      <c r="H89">
+        <v>3026.1817500000002</v>
+      </c>
+      <c r="I89">
+        <v>3033.82384</v>
+      </c>
+      <c r="J89">
+        <v>113.388738</v>
+      </c>
+      <c r="K89">
+        <v>2139.7611099999999</v>
+      </c>
+      <c r="L89">
+        <f t="shared" si="3"/>
+        <v>4.2678014630152337</v>
+      </c>
+      <c r="M89">
+        <f t="shared" si="4"/>
+        <v>3.737485891731934</v>
+      </c>
+      <c r="N89">
+        <f t="shared" si="5"/>
+        <v>0.53031557128329965</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -2522,8 +4948,35 @@
       <c r="F90">
         <v>1.0995412737034809</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G90">
+        <v>126.919349</v>
+      </c>
+      <c r="H90">
+        <v>3011.9945400000001</v>
+      </c>
+      <c r="I90">
+        <v>3038.83961</v>
+      </c>
+      <c r="J90">
+        <v>112.105031</v>
+      </c>
+      <c r="K90">
+        <v>2147.9298399999998</v>
+      </c>
+      <c r="L90">
+        <f t="shared" si="3"/>
+        <v>4.2137974459940422</v>
+      </c>
+      <c r="M90">
+        <f t="shared" si="4"/>
+        <v>3.6890736395265029</v>
+      </c>
+      <c r="N90">
+        <f t="shared" si="5"/>
+        <v>0.52472380646753924</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -2542,8 +4995,35 @@
       <c r="F91">
         <v>1.1079285716212564</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G91">
+        <v>113.08325000000001</v>
+      </c>
+      <c r="H91">
+        <v>3053.2020299999999</v>
+      </c>
+      <c r="I91">
+        <v>3044.1785399999999</v>
+      </c>
+      <c r="J91">
+        <v>110.09602099999999</v>
+      </c>
+      <c r="K91">
+        <v>2158.2878900000001</v>
+      </c>
+      <c r="L91">
+        <f t="shared" si="3"/>
+        <v>3.7037591646039885</v>
+      </c>
+      <c r="M91">
+        <f t="shared" si="4"/>
+        <v>3.6166085383415125</v>
+      </c>
+      <c r="N91">
+        <f t="shared" si="5"/>
+        <v>8.7150626262475939E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -2562,8 +5042,35 @@
       <c r="F92">
         <v>1.1160365438071953</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G92">
+        <v>94.995516899999998</v>
+      </c>
+      <c r="H92">
+        <v>3087.7042200000001</v>
+      </c>
+      <c r="I92">
+        <v>3049.67749</v>
+      </c>
+      <c r="J92">
+        <v>107.79573600000001</v>
+      </c>
+      <c r="K92">
+        <v>2165.4307600000002</v>
+      </c>
+      <c r="L92">
+        <f t="shared" si="3"/>
+        <v>3.0765743779694028</v>
+      </c>
+      <c r="M92">
+        <f t="shared" si="4"/>
+        <v>3.5346601846741508</v>
+      </c>
+      <c r="N92">
+        <f t="shared" si="5"/>
+        <v>-0.45808580670474797</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>92</v>
       </c>
@@ -2582,8 +5089,35 @@
       <c r="F93">
         <v>1.1331769998492991</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G93">
+        <v>78.657306599999998</v>
+      </c>
+      <c r="H93">
+        <v>3105.1590500000002</v>
+      </c>
+      <c r="I93">
+        <v>3055.7842599999999</v>
+      </c>
+      <c r="J93">
+        <v>105.10323699999999</v>
+      </c>
+      <c r="K93">
+        <v>2174.1989699999999</v>
+      </c>
+      <c r="L93">
+        <f t="shared" si="3"/>
+        <v>2.5331168334195313</v>
+      </c>
+      <c r="M93">
+        <f t="shared" si="4"/>
+        <v>3.4394848607538804</v>
+      </c>
+      <c r="N93">
+        <f t="shared" si="5"/>
+        <v>-0.90636802733434907</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -2602,8 +5136,35 @@
       <c r="F94">
         <v>1.1610697743166487</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G94">
+        <v>72.367058400000005</v>
+      </c>
+      <c r="H94">
+        <v>3110.4208899999999</v>
+      </c>
+      <c r="I94">
+        <v>3063.6067800000001</v>
+      </c>
+      <c r="J94">
+        <v>103.505313</v>
+      </c>
+      <c r="K94">
+        <v>2181.7535600000001</v>
+      </c>
+      <c r="L94">
+        <f t="shared" si="3"/>
+        <v>2.3266001920402486</v>
+      </c>
+      <c r="M94">
+        <f t="shared" si="4"/>
+        <v>3.3785443248039817</v>
+      </c>
+      <c r="N94">
+        <f t="shared" si="5"/>
+        <v>-1.0519441327637331</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>94</v>
       </c>
@@ -2622,8 +5183,35 @@
       <c r="F95">
         <v>1.1708176983026319</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G95">
+        <v>66.937347599999995</v>
+      </c>
+      <c r="H95">
+        <v>3109.5878899999998</v>
+      </c>
+      <c r="I95">
+        <v>3071.42931</v>
+      </c>
+      <c r="J95">
+        <v>101.934954</v>
+      </c>
+      <c r="K95">
+        <v>2192.76271</v>
+      </c>
+      <c r="L95">
+        <f t="shared" si="3"/>
+        <v>2.1526115346429395</v>
+      </c>
+      <c r="M95">
+        <f t="shared" si="4"/>
+        <v>3.3188116577555222</v>
+      </c>
+      <c r="N95">
+        <f t="shared" si="5"/>
+        <v>-1.1662001231125827</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -2642,8 +5230,35 @@
       <c r="F96">
         <v>1.166856231514332</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G96">
+        <v>65.304978199999994</v>
+      </c>
+      <c r="H96">
+        <v>3108.6893700000001</v>
+      </c>
+      <c r="I96">
+        <v>3079.2518399999999</v>
+      </c>
+      <c r="J96">
+        <v>100.604471</v>
+      </c>
+      <c r="K96">
+        <v>2205.8731400000001</v>
+      </c>
+      <c r="L96">
+        <f t="shared" si="3"/>
+        <v>2.1007238236865073</v>
+      </c>
+      <c r="M96">
+        <f t="shared" si="4"/>
+        <v>3.2671725544864825</v>
+      </c>
+      <c r="N96">
+        <f t="shared" si="5"/>
+        <v>-1.1664487307999751</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>96</v>
       </c>
@@ -2661,6 +5276,33 @@
       </c>
       <c r="F97">
         <v>1.1745783994521986</v>
+      </c>
+      <c r="G97">
+        <v>66.771159600000004</v>
+      </c>
+      <c r="H97">
+        <v>3107.0065399999999</v>
+      </c>
+      <c r="I97">
+        <v>3087.0743600000001</v>
+      </c>
+      <c r="J97">
+        <v>99.487372199999996</v>
+      </c>
+      <c r="K97">
+        <v>2217.7811499999998</v>
+      </c>
+      <c r="L97">
+        <f t="shared" si="3"/>
+        <v>2.149051144256684</v>
+      </c>
+      <c r="M97">
+        <f t="shared" si="4"/>
+        <v>3.2227073467708758</v>
+      </c>
+      <c r="N97">
+        <f t="shared" si="5"/>
+        <v>-1.0736562025141918</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed annualization problem in output potential for DK
</commit_message>
<xml_diff>
--- a/data/monaData.xlsx
+++ b/data/monaData.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\srv9dnbfil002\userhome\cjw\Documents\Inflation cluster\Semi-structurcal model of inflation dynamics\Data\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DN\Documents\inflationCycle\replication-hasenzagl-et-al-2020\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E17572-3091-422F-B6DA-B78C397C9718}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11010" xr2:uid="{3893118A-CCCC-4227-9FE2-63195E760603}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11010"/>
   </bookViews>
   <sheets>
     <sheet name="Ark2" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,12 +24,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Christoffer Jessen Weissert</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{721C1597-9E54-4385-9BBE-F8569B95D800}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -60,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
   <si>
     <t>fy_gab</t>
   </si>
@@ -387,12 +386,15 @@
   </si>
   <si>
     <t>fy_str</t>
+  </si>
+  <si>
+    <t>fy_str_unA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -743,16 +745,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B36B7F14-513A-48A1-91F4-A424ABF8C6B9}">
-  <dimension ref="A1:N97"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>97</v>
       </c>
@@ -792,8 +794,11 @@
       <c r="N1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -839,8 +844,12 @@
         <f>L2-M2</f>
         <v>-1.2390620377607346</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2">
+        <f>K2/4</f>
+        <v>397.84005250000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -886,8 +895,12 @@
         <f t="shared" ref="N3:N66" si="2">L3-M3</f>
         <v>-1.1244561821625974</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3">
+        <f t="shared" ref="O3:O66" si="3">K3/4</f>
+        <v>400.05921000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -933,8 +946,12 @@
         <f t="shared" si="2"/>
         <v>-1.0997805033927435</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4">
+        <f t="shared" si="3"/>
+        <v>402.23707250000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -980,8 +997,12 @@
         <f t="shared" si="2"/>
         <v>-1.0105866801895562</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5">
+        <f t="shared" si="3"/>
+        <v>404.53549249999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1027,8 +1048,12 @@
         <f t="shared" si="2"/>
         <v>-0.9631013393595218</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6">
+        <f t="shared" si="3"/>
+        <v>407.3992025</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1074,8 +1099,12 @@
         <f t="shared" si="2"/>
         <v>-0.94763862097018059</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7">
+        <f t="shared" si="3"/>
+        <v>409.81705749999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1121,8 +1150,12 @@
         <f t="shared" si="2"/>
         <v>-0.9431847473338566</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8">
+        <f t="shared" si="3"/>
+        <v>412.07533999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1168,8 +1201,12 @@
         <f t="shared" si="2"/>
         <v>-0.9657097546416944</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9">
+        <f t="shared" si="3"/>
+        <v>414.2393975</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1215,8 +1252,12 @@
         <f t="shared" si="2"/>
         <v>-0.97360032234168603</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10">
+        <f t="shared" si="3"/>
+        <v>416.18380999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1262,8 +1303,12 @@
         <f t="shared" si="2"/>
         <v>-1.0270567910834369</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11">
+        <f t="shared" si="3"/>
+        <v>418.32660750000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1309,8 +1354,12 @@
         <f t="shared" si="2"/>
         <v>-1.0105298095468571</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12">
+        <f t="shared" si="3"/>
+        <v>420.40698500000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1356,8 +1405,12 @@
         <f t="shared" si="2"/>
         <v>-1.0019929473780209</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O13">
+        <f t="shared" si="3"/>
+        <v>422.535145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1403,8 +1456,12 @@
         <f t="shared" si="2"/>
         <v>-0.78756422230656487</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14">
+        <f t="shared" si="3"/>
+        <v>424.414535</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1450,8 +1507,12 @@
         <f t="shared" si="2"/>
         <v>-0.74308486941504714</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15">
+        <f t="shared" si="3"/>
+        <v>426.01174250000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1497,8 +1558,12 @@
         <f t="shared" si="2"/>
         <v>-0.60654533384188269</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O16">
+        <f t="shared" si="3"/>
+        <v>427.68350249999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1544,8 +1609,12 @@
         <f t="shared" si="2"/>
         <v>-0.40557677942409143</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O17">
+        <f t="shared" si="3"/>
+        <v>429.20251000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1591,8 +1660,12 @@
         <f t="shared" si="2"/>
         <v>-7.1937272538852071E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18">
+        <f t="shared" si="3"/>
+        <v>430.76032249999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1638,8 +1711,12 @@
         <f t="shared" si="2"/>
         <v>0.21445195817339791</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O19">
+        <f t="shared" si="3"/>
+        <v>431.85043250000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1685,8 +1762,12 @@
         <f t="shared" si="2"/>
         <v>0.38191068321665522</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O20">
+        <f t="shared" si="3"/>
+        <v>433.15490999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1732,8 +1813,12 @@
         <f t="shared" si="2"/>
         <v>0.66160994812938423</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O21">
+        <f t="shared" si="3"/>
+        <v>434.66021749999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1779,8 +1864,12 @@
         <f t="shared" si="2"/>
         <v>0.66614525867001984</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O22">
+        <f t="shared" si="3"/>
+        <v>435.60929249999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1826,8 +1915,12 @@
         <f t="shared" si="2"/>
         <v>0.65129429784308535</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O23">
+        <f t="shared" si="3"/>
+        <v>437.02343500000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1873,8 +1966,12 @@
         <f t="shared" si="2"/>
         <v>0.60631401506079552</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O24">
+        <f t="shared" si="3"/>
+        <v>438.45845250000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1920,8 +2017,12 @@
         <f t="shared" si="2"/>
         <v>0.68773737806559687</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O25">
+        <f t="shared" si="3"/>
+        <v>440.00835499999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1967,8 +2068,12 @@
         <f t="shared" si="2"/>
         <v>0.52596233091868871</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O26">
+        <f t="shared" si="3"/>
+        <v>441.41454750000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2014,8 +2119,12 @@
         <f t="shared" si="2"/>
         <v>0.47476120383828757</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O27">
+        <f t="shared" si="3"/>
+        <v>442.87119000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -2061,8 +2170,12 @@
         <f t="shared" si="2"/>
         <v>0.31656656463677013</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O28">
+        <f t="shared" si="3"/>
+        <v>444.21087749999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -2108,8 +2221,12 @@
         <f t="shared" si="2"/>
         <v>0.13821734351032156</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O29">
+        <f t="shared" si="3"/>
+        <v>445.63055250000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -2155,8 +2272,12 @@
         <f t="shared" si="2"/>
         <v>-0.2242135457321659</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O30">
+        <f t="shared" si="3"/>
+        <v>447.09718750000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -2202,8 +2323,12 @@
         <f t="shared" si="2"/>
         <v>-0.41991271666707686</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O31">
+        <f t="shared" si="3"/>
+        <v>449.22668750000003</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -2249,8 +2374,12 @@
         <f t="shared" si="2"/>
         <v>-0.57219160836234462</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O32">
+        <f t="shared" si="3"/>
+        <v>450.94409250000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -2296,8 +2425,12 @@
         <f t="shared" si="2"/>
         <v>-0.79655978688135942</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O33">
+        <f t="shared" si="3"/>
+        <v>452.52138000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -2343,8 +2476,12 @@
         <f t="shared" si="2"/>
         <v>-1.0380480715480691</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O34">
+        <f t="shared" si="3"/>
+        <v>454.42874749999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -2390,8 +2527,12 @@
         <f t="shared" si="2"/>
         <v>-1.204804651532557</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O35">
+        <f t="shared" si="3"/>
+        <v>456.06399249999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -2437,8 +2578,12 @@
         <f t="shared" si="2"/>
         <v>-1.377924761748623</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O36">
+        <f t="shared" si="3"/>
+        <v>457.66524500000003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -2484,8 +2629,12 @@
         <f t="shared" si="2"/>
         <v>-1.6439472242562911</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O37">
+        <f t="shared" si="3"/>
+        <v>459.376035</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -2531,8 +2680,12 @@
         <f t="shared" si="2"/>
         <v>-1.9392394593351128</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O38">
+        <f t="shared" si="3"/>
+        <v>461.120655</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2578,8 +2731,12 @@
         <f t="shared" si="2"/>
         <v>-2.1627883409367077</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O39">
+        <f t="shared" si="3"/>
+        <v>462.52734249999997</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -2625,8 +2782,12 @@
         <f t="shared" si="2"/>
         <v>-2.0670776590991653</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O40">
+        <f t="shared" si="3"/>
+        <v>463.99572999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -2672,8 +2833,12 @@
         <f t="shared" si="2"/>
         <v>-1.7054949987919157</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O41">
+        <f t="shared" si="3"/>
+        <v>465.16046</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -2719,8 +2884,12 @@
         <f t="shared" si="2"/>
         <v>-0.95226497707692914</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O42">
+        <f t="shared" si="3"/>
+        <v>466.06598500000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -2766,8 +2935,12 @@
         <f t="shared" si="2"/>
         <v>4.7210585596184629E-3</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O43">
+        <f t="shared" si="3"/>
+        <v>466.7207075</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2813,8 +2986,12 @@
         <f t="shared" si="2"/>
         <v>0.51048140232895012</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O44">
+        <f t="shared" si="3"/>
+        <v>467.41355499999997</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2860,8 +3037,12 @@
         <f t="shared" si="2"/>
         <v>0.90128864606555137</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O45">
+        <f t="shared" si="3"/>
+        <v>467.85808750000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -2907,8 +3088,12 @@
         <f t="shared" si="2"/>
         <v>1.1283395682278403</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O46">
+        <f t="shared" si="3"/>
+        <v>468.11463500000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -2954,8 +3139,12 @@
         <f t="shared" si="2"/>
         <v>1.0676741437491142</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O47">
+        <f t="shared" si="3"/>
+        <v>468.71318250000002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -3001,8 +3190,12 @@
         <f t="shared" si="2"/>
         <v>1.0667423021308746</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O48">
+        <f t="shared" si="3"/>
+        <v>469.35236500000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -3048,8 +3241,12 @@
         <f t="shared" si="2"/>
         <v>1.0294033519657306</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O49">
+        <f t="shared" si="3"/>
+        <v>469.89094499999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -3095,8 +3292,12 @@
         <f t="shared" si="2"/>
         <v>0.95602721003838997</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O50">
+        <f t="shared" si="3"/>
+        <v>470.2822425</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -3142,8 +3343,12 @@
         <f t="shared" si="2"/>
         <v>0.88168436172923226</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O51">
+        <f t="shared" si="3"/>
+        <v>470.94596999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -3189,8 +3394,12 @@
         <f t="shared" si="2"/>
         <v>0.90086139596004777</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O52">
+        <f t="shared" si="3"/>
+        <v>471.43303750000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -3236,8 +3445,12 @@
         <f t="shared" si="2"/>
         <v>0.72303241682658559</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O53">
+        <f t="shared" si="3"/>
+        <v>471.78127499999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -3283,8 +3496,12 @@
         <f t="shared" si="2"/>
         <v>0.87523606476952498</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O54">
+        <f t="shared" si="3"/>
+        <v>472.30099749999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -3330,8 +3547,12 @@
         <f t="shared" si="2"/>
         <v>1.0848673957427843</v>
       </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O55">
+        <f t="shared" si="3"/>
+        <v>472.97562749999997</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -3377,8 +3598,12 @@
         <f t="shared" si="2"/>
         <v>1.0902941851860595</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O56">
+        <f t="shared" si="3"/>
+        <v>473.62801000000002</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -3424,8 +3649,12 @@
         <f t="shared" si="2"/>
         <v>1.0269745525177232</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O57">
+        <f t="shared" si="3"/>
+        <v>474.28351750000002</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -3471,8 +3700,12 @@
         <f t="shared" si="2"/>
         <v>0.99809929020357124</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O58">
+        <f t="shared" si="3"/>
+        <v>475.13083749999998</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -3518,8 +3751,12 @@
         <f t="shared" si="2"/>
         <v>1.0044142822232143</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O59">
+        <f t="shared" si="3"/>
+        <v>475.82875000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -3565,8 +3802,12 @@
         <f t="shared" si="2"/>
         <v>0.90453781635183894</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O60">
+        <f t="shared" si="3"/>
+        <v>476.87474750000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -3612,8 +3853,12 @@
         <f t="shared" si="2"/>
         <v>0.85735032647582887</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O61">
+        <f t="shared" si="3"/>
+        <v>477.94468499999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -3659,8 +3904,12 @@
         <f t="shared" si="2"/>
         <v>0.56072448046203682</v>
       </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O62">
+        <f t="shared" si="3"/>
+        <v>479.16979500000002</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -3706,8 +3955,12 @@
         <f t="shared" si="2"/>
         <v>0.46995053599753334</v>
       </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O63">
+        <f t="shared" si="3"/>
+        <v>480.47079000000002</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -3753,8 +4006,12 @@
         <f t="shared" si="2"/>
         <v>0.42109681825200962</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O64">
+        <f t="shared" si="3"/>
+        <v>481.920435</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -3800,8 +4057,12 @@
         <f t="shared" si="2"/>
         <v>0.40051186253101134</v>
       </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O65">
+        <f t="shared" si="3"/>
+        <v>483.45997499999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -3847,8 +4108,12 @@
         <f t="shared" si="2"/>
         <v>0.36527307612481863</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O66">
+        <f t="shared" si="3"/>
+        <v>485.11340749999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -3883,19 +4148,23 @@
         <v>1947.43595</v>
       </c>
       <c r="L67">
-        <f t="shared" ref="L67:L97" si="3">G67/H67*100</f>
+        <f t="shared" ref="L67:L97" si="4">G67/H67*100</f>
         <v>4.2530013275689003</v>
       </c>
       <c r="M67">
-        <f t="shared" ref="M67:M97" si="4">J67/I67*100</f>
+        <f t="shared" ref="M67:M97" si="5">J67/I67*100</f>
         <v>3.906781372867993</v>
       </c>
       <c r="N67">
-        <f t="shared" ref="N67:N97" si="5">L67-M67</f>
+        <f t="shared" ref="N67:N97" si="6">L67-M67</f>
         <v>0.34621995470090727</v>
       </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O67">
+        <f t="shared" ref="O67:O97" si="7">K67/4</f>
+        <v>486.85898750000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -3930,19 +4199,23 @@
         <v>1954.6157499999999</v>
       </c>
       <c r="L68">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.0765532407113181</v>
       </c>
       <c r="M68">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.8586392077994525</v>
       </c>
       <c r="N68">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.21791403291186562</v>
       </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O68">
+        <f t="shared" si="7"/>
+        <v>488.65393749999998</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -3977,19 +4250,23 @@
         <v>1961.71046</v>
       </c>
       <c r="L69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.9571706500677228</v>
       </c>
       <c r="M69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.8525305708321431</v>
       </c>
       <c r="N69">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.10464007923557972</v>
       </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O69">
+        <f t="shared" si="7"/>
+        <v>490.427615</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -4024,19 +4301,23 @@
         <v>1969.31062</v>
       </c>
       <c r="L70">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.8587625780231138</v>
       </c>
       <c r="M70">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.8447116221839965</v>
       </c>
       <c r="N70">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.4050955839117307E-2</v>
       </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O70">
+        <f t="shared" si="7"/>
+        <v>492.32765499999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -4071,19 +4352,23 @@
         <v>1977.65751</v>
       </c>
       <c r="L71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.7541571056899627</v>
       </c>
       <c r="M71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.8544038835342604</v>
       </c>
       <c r="N71">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.1002467778442977</v>
       </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O71">
+        <f t="shared" si="7"/>
+        <v>494.4143775</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -4118,19 +4403,23 @@
         <v>1985.71703</v>
       </c>
       <c r="L72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.7045164998973932</v>
       </c>
       <c r="M72">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.0147119126354163</v>
       </c>
       <c r="N72">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.31019541273802309</v>
       </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O72">
+        <f t="shared" si="7"/>
+        <v>496.42925750000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -4165,19 +4454,23 @@
         <v>1998.2604100000001</v>
       </c>
       <c r="L73">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.7519650995332929</v>
       </c>
       <c r="M73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.1605550768554016</v>
       </c>
       <c r="N73">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.40858997732210867</v>
       </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O73">
+        <f t="shared" si="7"/>
+        <v>499.56510250000002</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -4212,19 +4505,23 @@
         <v>2007.52189</v>
       </c>
       <c r="L74">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.8453094397184668</v>
       </c>
       <c r="M74">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.2748578218226774</v>
       </c>
       <c r="N74">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.42954838210421054</v>
       </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O74">
+        <f t="shared" si="7"/>
+        <v>501.8804725</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -4259,19 +4556,23 @@
         <v>2016.5584899999999</v>
       </c>
       <c r="L75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.8396925142642298</v>
       </c>
       <c r="M75">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.3475559195005076</v>
       </c>
       <c r="N75">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.50786340523627782</v>
       </c>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O75">
+        <f t="shared" si="7"/>
+        <v>504.13962249999997</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -4306,19 +4607,23 @@
         <v>2027.18523</v>
       </c>
       <c r="L76">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.8971812425647943</v>
       </c>
       <c r="M76">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.315982332032883</v>
       </c>
       <c r="N76">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.41880108946808869</v>
       </c>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O76">
+        <f t="shared" si="7"/>
+        <v>506.79630750000001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -4353,19 +4658,23 @@
         <v>2037.83086</v>
       </c>
       <c r="L77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.7878700338942868</v>
       </c>
       <c r="M77">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.2517730325387815</v>
       </c>
       <c r="N77">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.46390299864449469</v>
       </c>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O77">
+        <f t="shared" si="7"/>
+        <v>509.45771500000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -4400,19 +4709,23 @@
         <v>2047.9069199999999</v>
       </c>
       <c r="L78">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.6657910780792129</v>
       </c>
       <c r="M78">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.2008828899861452</v>
       </c>
       <c r="N78">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.53509181190693234</v>
       </c>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O78">
+        <f t="shared" si="7"/>
+        <v>511.97672999999998</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -4447,19 +4760,23 @@
         <v>2059.49325</v>
       </c>
       <c r="L79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.5616764601107334</v>
       </c>
       <c r="M79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.156696772144544</v>
       </c>
       <c r="N79">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.59502031203381067</v>
       </c>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O79">
+        <f t="shared" si="7"/>
+        <v>514.8733125</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -4494,19 +4811,23 @@
         <v>2068.0679</v>
       </c>
       <c r="L80">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.4736079873409813</v>
       </c>
       <c r="M80">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.1033960281901729</v>
       </c>
       <c r="N80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.6297880408491916</v>
       </c>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O80">
+        <f t="shared" si="7"/>
+        <v>517.016975</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -4541,19 +4862,23 @@
         <v>2079.4666999999999</v>
       </c>
       <c r="L81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.459335725457279</v>
       </c>
       <c r="M81">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.0449868862785436</v>
       </c>
       <c r="N81">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.58565116082126467</v>
       </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O81">
+        <f t="shared" si="7"/>
+        <v>519.86667499999999</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -4588,19 +4913,23 @@
         <v>2088.9252799999999</v>
       </c>
       <c r="L82">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.3831213336712898</v>
       </c>
       <c r="M82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.9981963923839277</v>
       </c>
       <c r="N82">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.6150750587126379</v>
       </c>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O82">
+        <f t="shared" si="7"/>
+        <v>522.23131999999998</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -4635,19 +4964,23 @@
         <v>2097.8122899999998</v>
       </c>
       <c r="L83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.3325647994903078</v>
       </c>
       <c r="M83">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.9534250502319623</v>
       </c>
       <c r="N83">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.62086025074165452</v>
       </c>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O83">
+        <f t="shared" si="7"/>
+        <v>524.45307249999996</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -4682,19 +5015,23 @@
         <v>2105.8855400000002</v>
       </c>
       <c r="L84">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.3965835142615872</v>
       </c>
       <c r="M84">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.9164465983727683</v>
       </c>
       <c r="N84">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.5198630841111811</v>
       </c>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O84">
+        <f t="shared" si="7"/>
+        <v>526.47138500000005</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -4729,19 +5066,23 @@
         <v>2113.5398599999999</v>
       </c>
       <c r="L85">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.4514286665297038</v>
       </c>
       <c r="M85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.8805516787420551</v>
       </c>
       <c r="N85">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.42912301221235127</v>
       </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O85">
+        <f t="shared" si="7"/>
+        <v>528.38496499999997</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -4776,19 +5117,23 @@
         <v>2118.0178000000001</v>
       </c>
       <c r="L86">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.5164810335504497</v>
       </c>
       <c r="M86">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.8434184281310637</v>
       </c>
       <c r="N86">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.32693739458061399</v>
       </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O86">
+        <f t="shared" si="7"/>
+        <v>529.50445000000002</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -4823,19 +5168,23 @@
         <v>2122.3657800000001</v>
       </c>
       <c r="L87">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.9974567317322593</v>
       </c>
       <c r="M87">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.8449206077187501</v>
       </c>
       <c r="N87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.1525361240135092</v>
       </c>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O87">
+        <f t="shared" si="7"/>
+        <v>530.59144500000002</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -4870,19 +5219,23 @@
         <v>2131.09256</v>
       </c>
       <c r="L88">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.5512441598450772</v>
       </c>
       <c r="M88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.7894961375756804</v>
       </c>
       <c r="N88">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.76174802226939686</v>
       </c>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O88">
+        <f t="shared" si="7"/>
+        <v>532.77314000000001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -4917,19 +5270,23 @@
         <v>2139.7611099999999</v>
       </c>
       <c r="L89">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.2678014630152337</v>
       </c>
       <c r="M89">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.737485891731934</v>
       </c>
       <c r="N89">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.53031557128329965</v>
       </c>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O89">
+        <f t="shared" si="7"/>
+        <v>534.94027749999998</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -4964,19 +5321,23 @@
         <v>2147.9298399999998</v>
       </c>
       <c r="L90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.2137974459940422</v>
       </c>
       <c r="M90">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.6890736395265029</v>
       </c>
       <c r="N90">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.52472380646753924</v>
       </c>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O90">
+        <f t="shared" si="7"/>
+        <v>536.98245999999995</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -5011,19 +5372,23 @@
         <v>2158.2878900000001</v>
       </c>
       <c r="L91">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.7037591646039885</v>
       </c>
       <c r="M91">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.6166085383415125</v>
       </c>
       <c r="N91">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8.7150626262475939E-2</v>
       </c>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O91">
+        <f t="shared" si="7"/>
+        <v>539.57197250000002</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -5058,19 +5423,23 @@
         <v>2165.4307600000002</v>
       </c>
       <c r="L92">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.0765743779694028</v>
       </c>
       <c r="M92">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.5346601846741508</v>
       </c>
       <c r="N92">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.45808580670474797</v>
       </c>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O92">
+        <f t="shared" si="7"/>
+        <v>541.35769000000005</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>92</v>
       </c>
@@ -5105,19 +5474,23 @@
         <v>2174.1989699999999</v>
       </c>
       <c r="L93">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.5331168334195313</v>
       </c>
       <c r="M93">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.4394848607538804</v>
       </c>
       <c r="N93">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.90636802733434907</v>
       </c>
-    </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O93">
+        <f t="shared" si="7"/>
+        <v>543.54974249999998</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -5152,19 +5525,23 @@
         <v>2181.7535600000001</v>
       </c>
       <c r="L94">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.3266001920402486</v>
       </c>
       <c r="M94">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.3785443248039817</v>
       </c>
       <c r="N94">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-1.0519441327637331</v>
       </c>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O94">
+        <f t="shared" si="7"/>
+        <v>545.43839000000003</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>94</v>
       </c>
@@ -5199,19 +5576,23 @@
         <v>2192.76271</v>
       </c>
       <c r="L95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.1526115346429395</v>
       </c>
       <c r="M95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.3188116577555222</v>
       </c>
       <c r="N95">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-1.1662001231125827</v>
       </c>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O95">
+        <f t="shared" si="7"/>
+        <v>548.19067749999999</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -5246,19 +5627,23 @@
         <v>2205.8731400000001</v>
       </c>
       <c r="L96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.1007238236865073</v>
       </c>
       <c r="M96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.2671725544864825</v>
       </c>
       <c r="N96">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-1.1664487307999751</v>
       </c>
-    </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O96">
+        <f t="shared" si="7"/>
+        <v>551.46828500000004</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>96</v>
       </c>
@@ -5293,16 +5678,20 @@
         <v>2217.7811499999998</v>
       </c>
       <c r="L97">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.149051144256684</v>
       </c>
       <c r="M97">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.2227073467708758</v>
       </c>
       <c r="N97">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-1.0736562025141918</v>
+      </c>
+      <c r="O97">
+        <f t="shared" si="7"/>
+        <v>554.44528749999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Danish data from MONA
</commit_message>
<xml_diff>
--- a/data/monaData.xlsx
+++ b/data/monaData.xlsx
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
   <si>
     <t>fy_gab</t>
   </si>
@@ -389,6 +389,12 @@
   </si>
   <si>
     <t>fy_str_unA</t>
+  </si>
+  <si>
+    <t>fy_unA</t>
+  </si>
+  <si>
+    <t>pcpdkeu_Yrate</t>
   </si>
 </sst>
 </file>
@@ -746,15 +752,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O97"/>
+  <dimension ref="A1:Q97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17:Q97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>97</v>
       </c>
@@ -797,8 +803,14 @@
       <c r="O1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -848,8 +860,12 @@
         <f>K2/4</f>
         <v>397.84005250000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P2">
+        <f>B2/4</f>
+        <v>399.95499999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -899,8 +915,12 @@
         <f t="shared" ref="O3:O66" si="3">K3/4</f>
         <v>400.05921000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P3">
+        <f t="shared" ref="P3:P66" si="4">B3/4</f>
+        <v>402.02024999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -950,8 +970,12 @@
         <f t="shared" si="3"/>
         <v>402.23707250000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P4">
+        <f t="shared" si="4"/>
+        <v>404.505</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1001,8 +1025,12 @@
         <f t="shared" si="3"/>
         <v>404.53549249999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P5">
+        <f t="shared" si="4"/>
+        <v>410.16325000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1052,8 +1080,16 @@
         <f t="shared" si="3"/>
         <v>407.3992025</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P6">
+        <f t="shared" si="4"/>
+        <v>414.16264782665729</v>
+      </c>
+      <c r="Q6">
+        <f>F6/F2*100-100</f>
+        <v>2.8320110789358495</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1103,8 +1139,16 @@
         <f t="shared" si="3"/>
         <v>409.81705749999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P7">
+        <f t="shared" si="4"/>
+        <v>418.87737267657445</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" ref="Q7:Q70" si="5">F7/F3*100-100</f>
+        <v>2.8446006807234312</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1154,8 +1198,16 @@
         <f t="shared" si="3"/>
         <v>412.07533999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P8">
+        <f t="shared" si="4"/>
+        <v>420.03467182112092</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="5"/>
+        <v>2.5643494520912498</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1205,8 +1257,16 @@
         <f t="shared" si="3"/>
         <v>414.2393975</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P9">
+        <f t="shared" si="4"/>
+        <v>424.14172989204019</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="5"/>
+        <v>2.6058629873844552</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1256,8 +1316,16 @@
         <f t="shared" si="3"/>
         <v>416.18380999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P10">
+        <f t="shared" si="4"/>
+        <v>419.53671667627532</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="5"/>
+        <v>2.3057662327640998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1307,8 +1375,16 @@
         <f t="shared" si="3"/>
         <v>418.32660750000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P11">
+        <f t="shared" si="4"/>
+        <v>421.5849252272954</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="5"/>
+        <v>2.5552785864677503</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1358,8 +1434,16 @@
         <f t="shared" si="3"/>
         <v>420.40698500000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P12">
+        <f t="shared" si="4"/>
+        <v>425.36995260441074</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="5"/>
+        <v>2.3553525374408366</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1409,8 +1493,16 @@
         <f t="shared" si="3"/>
         <v>422.535145</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P13">
+        <f t="shared" si="4"/>
+        <v>424.53115291785957</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="5"/>
+        <v>1.9874608269834226</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1460,8 +1552,16 @@
         <f t="shared" si="3"/>
         <v>424.414535</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P14">
+        <f t="shared" si="4"/>
+        <v>424.38876224703091</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="5"/>
+        <v>2.4083105810524899</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1511,8 +1611,16 @@
         <f t="shared" si="3"/>
         <v>426.01174250000003</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P15">
+        <f t="shared" si="4"/>
+        <v>424.34647201804802</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="5"/>
+        <v>2.0993743452083464</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1562,8 +1670,16 @@
         <f t="shared" si="3"/>
         <v>427.68350249999997</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P16">
+        <f t="shared" si="4"/>
+        <v>425.78942588532556</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="5"/>
+        <v>2.3628793668459593</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1610,11 +1726,19 @@
         <v>-0.40557677942409143</v>
       </c>
       <c r="O17">
-        <f t="shared" si="3"/>
+        <f>K17/4</f>
         <v>429.20251000000002</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P17">
+        <f t="shared" si="4"/>
+        <v>424.38428145154364</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="5"/>
+        <v>2.6567145095871325</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1664,8 +1788,16 @@
         <f t="shared" si="3"/>
         <v>430.76032249999997</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P18">
+        <f t="shared" si="4"/>
+        <v>426.65842163047449</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="5"/>
+        <v>2.7876331661756097</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1715,8 +1847,16 @@
         <f t="shared" si="3"/>
         <v>431.85043250000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P19">
+        <f t="shared" si="4"/>
+        <v>422.69031770012788</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="5"/>
+        <v>2.2322014483090697</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1766,8 +1906,16 @@
         <f t="shared" si="3"/>
         <v>433.15490999999997</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P20">
+        <f t="shared" si="4"/>
+        <v>424.14213549532633</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="5"/>
+        <v>1.6316903369301201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1817,8 +1965,16 @@
         <f t="shared" si="3"/>
         <v>434.66021749999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P21">
+        <f t="shared" si="4"/>
+        <v>432.04408798640651</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="5"/>
+        <v>1.2765601306205809</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1868,8 +2024,16 @@
         <f t="shared" si="3"/>
         <v>435.60929249999998</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P22">
+        <f t="shared" si="4"/>
+        <v>434.12483578467658</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="5"/>
+        <v>0.66597011290178898</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1919,8 +2083,16 @@
         <f t="shared" si="3"/>
         <v>437.02343500000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P23">
+        <f t="shared" si="4"/>
+        <v>436.70939408054096</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="5"/>
+        <v>0.81276189937202048</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1970,8 +2142,16 @@
         <f t="shared" si="3"/>
         <v>438.45845250000002</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P24">
+        <f t="shared" si="4"/>
+        <v>437.73833983170829</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="5"/>
+        <v>0.95036461825839069</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -2021,8 +2201,16 @@
         <f t="shared" si="3"/>
         <v>440.00835499999999</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P25">
+        <f t="shared" si="4"/>
+        <v>442.46988937678321</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="5"/>
+        <v>1.162089098747316</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -2072,8 +2260,16 @@
         <f t="shared" si="3"/>
         <v>441.41454750000003</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P26">
+        <f t="shared" si="4"/>
+        <v>440.86389390977831</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="5"/>
+        <v>1.0690724719377727</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2123,8 +2319,16 @@
         <f t="shared" si="3"/>
         <v>442.87119000000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P27">
+        <f t="shared" si="4"/>
+        <v>449.54388061270527</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="5"/>
+        <v>1.5530667045191819</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -2174,8 +2378,16 @@
         <f t="shared" si="3"/>
         <v>444.21087749999998</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P28">
+        <f t="shared" si="4"/>
+        <v>450.044603740019</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="5"/>
+        <v>2.1560535515357913</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -2225,8 +2437,16 @@
         <f t="shared" si="3"/>
         <v>445.63055250000002</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P29">
+        <f t="shared" si="4"/>
+        <v>451.50604982667647</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="5"/>
+        <v>2.0030822733889693</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -2276,8 +2496,16 @@
         <f t="shared" si="3"/>
         <v>447.09718750000002</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P30">
+        <f t="shared" si="4"/>
+        <v>457.18002117634103</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="5"/>
+        <v>1.9968159673120311</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -2327,8 +2555,16 @@
         <f t="shared" si="3"/>
         <v>449.22668750000003</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P31">
+        <f t="shared" si="4"/>
+        <v>470.81498115628392</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="5"/>
+        <v>1.9931684741141709</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -2378,8 +2614,16 @@
         <f t="shared" si="3"/>
         <v>450.94409250000001</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P32">
+        <f t="shared" si="4"/>
+        <v>467.67536966685446</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="5"/>
+        <v>1.7806372918343527</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -2429,8 +2673,16 @@
         <f t="shared" si="3"/>
         <v>452.52138000000002</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P33">
+        <f t="shared" si="4"/>
+        <v>466.40781629654992</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="5"/>
+        <v>1.6466949201847854</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -2480,8 +2732,16 @@
         <f t="shared" si="3"/>
         <v>454.42874749999999</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P34">
+        <f t="shared" si="4"/>
+        <v>467.95285824848651</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="5"/>
+        <v>1.8385367484820279</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -2531,8 +2791,16 @@
         <f t="shared" si="3"/>
         <v>456.06399249999998</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P35">
+        <f t="shared" si="4"/>
+        <v>465.85704250766031</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="5"/>
+        <v>1.5375056129182099</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -2582,8 +2850,16 @@
         <f t="shared" si="3"/>
         <v>457.66524500000003</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P36">
+        <f t="shared" si="4"/>
+        <v>470.23380171874754</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="5"/>
+        <v>1.0283380906707151</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -2633,8 +2909,16 @@
         <f t="shared" si="3"/>
         <v>459.376035</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P37">
+        <f t="shared" si="4"/>
+        <v>474.96418557379127</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="5"/>
+        <v>2.2852724245426543</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -2684,8 +2968,16 @@
         <f t="shared" si="3"/>
         <v>461.120655</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P38">
+        <f t="shared" si="4"/>
+        <v>474.76699008031318</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="5"/>
+        <v>3.1829215019694317</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2735,8 +3027,16 @@
         <f t="shared" si="3"/>
         <v>462.52734249999997</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P39">
+        <f t="shared" si="4"/>
+        <v>470.38611687500799</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" si="5"/>
+        <v>3.7032805044464538</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -2786,8 +3086,16 @@
         <f t="shared" si="3"/>
         <v>463.99572999999998</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P40">
+        <f t="shared" si="4"/>
+        <v>467.63837536775742</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="5"/>
+        <v>4.5504755636069518</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -2837,8 +3145,16 @@
         <f t="shared" si="3"/>
         <v>465.16046</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P41">
+        <f t="shared" si="4"/>
+        <v>456.59522282354374</v>
+      </c>
+      <c r="Q41">
+        <f t="shared" si="5"/>
+        <v>3.0290907463516987</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -2888,8 +3204,16 @@
         <f t="shared" si="3"/>
         <v>466.06598500000001</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P42">
+        <f t="shared" si="4"/>
+        <v>450.09601682374256</v>
+      </c>
+      <c r="Q42">
+        <f t="shared" si="5"/>
+        <v>1.6185749085576333</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -2939,8 +3263,16 @@
         <f t="shared" si="3"/>
         <v>466.7207075</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P43">
+        <f t="shared" si="4"/>
+        <v>441.37155063831676</v>
+      </c>
+      <c r="Q43">
+        <f t="shared" si="5"/>
+        <v>1.0707912896072713</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2990,8 +3322,16 @@
         <f t="shared" si="3"/>
         <v>467.41355499999997</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P44">
+        <f t="shared" si="4"/>
+        <v>442.89788339145127</v>
+      </c>
+      <c r="Q44">
+        <f t="shared" si="5"/>
+        <v>0.62979285887156777</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -3041,8 +3381,16 @@
         <f t="shared" si="3"/>
         <v>467.85808750000001</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P45">
+        <f t="shared" si="4"/>
+        <v>443.29950098233263</v>
+      </c>
+      <c r="Q45">
+        <f t="shared" si="5"/>
+        <v>0.99255033198379294</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -3092,8 +3440,16 @@
         <f t="shared" si="3"/>
         <v>468.11463500000002</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P46">
+        <f t="shared" si="4"/>
+        <v>447.12761957935817</v>
+      </c>
+      <c r="Q46">
+        <f t="shared" si="5"/>
+        <v>1.8963274104951466</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -3143,8 +3499,16 @@
         <f t="shared" si="3"/>
         <v>468.71318250000002</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P47">
+        <f t="shared" si="4"/>
+        <v>450.18393426737896</v>
+      </c>
+      <c r="Q47">
+        <f t="shared" si="5"/>
+        <v>2.0505215803546548</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -3194,8 +3558,16 @@
         <f t="shared" si="3"/>
         <v>469.35236500000002</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P48">
+        <f t="shared" si="4"/>
+        <v>457.32091470683025</v>
+      </c>
+      <c r="Q48">
+        <f t="shared" si="5"/>
+        <v>2.3487719986913191</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -3245,8 +3617,16 @@
         <f t="shared" si="3"/>
         <v>469.89094499999999</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P49">
+        <f t="shared" si="4"/>
+        <v>456.29173137122615</v>
+      </c>
+      <c r="Q49">
+        <f t="shared" si="5"/>
+        <v>2.4810514146719242</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -3296,8 +3676,16 @@
         <f t="shared" si="3"/>
         <v>470.2822425</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P50">
+        <f t="shared" si="4"/>
+        <v>457.28605565734921</v>
+      </c>
+      <c r="Q50">
+        <f t="shared" si="5"/>
+        <v>2.5559208031060052</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -3347,8 +3735,16 @@
         <f t="shared" si="3"/>
         <v>470.94596999999999</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P51">
+        <f t="shared" si="4"/>
+        <v>461.86922735133891</v>
+      </c>
+      <c r="Q51">
+        <f t="shared" si="5"/>
+        <v>2.9726135307838604</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -3398,8 +3794,16 @@
         <f t="shared" si="3"/>
         <v>471.43303750000001</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P52">
+        <f t="shared" si="4"/>
+        <v>456.12485665882713</v>
+      </c>
+      <c r="Q52">
+        <f t="shared" si="5"/>
+        <v>2.5382770187301702</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -3449,8 +3853,16 @@
         <f t="shared" si="3"/>
         <v>471.78127499999999</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P53">
+        <f t="shared" si="4"/>
+        <v>459.85238295888735</v>
+      </c>
+      <c r="Q53">
+        <f t="shared" si="5"/>
+        <v>2.5360348657623746</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -3500,8 +3912,16 @@
         <f t="shared" si="3"/>
         <v>472.30099749999999</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P54">
+        <f t="shared" si="4"/>
+        <v>459.53256841400321</v>
+      </c>
+      <c r="Q54">
+        <f t="shared" si="5"/>
+        <v>2.730574076856044</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -3551,8 +3971,16 @@
         <f t="shared" si="3"/>
         <v>472.97562749999997</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P55">
+        <f t="shared" si="4"/>
+        <v>459.87816965349032</v>
+      </c>
+      <c r="Q55">
+        <f t="shared" si="5"/>
+        <v>2.1571295422453005</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -3602,8 +4030,16 @@
         <f t="shared" si="3"/>
         <v>473.62801000000002</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P56">
+        <f t="shared" si="4"/>
+        <v>460.31023124544515</v>
+      </c>
+      <c r="Q56">
+        <f t="shared" si="5"/>
+        <v>2.4452171545249541</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -3653,8 +4089,16 @@
         <f t="shared" si="3"/>
         <v>474.28351750000002</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P57">
+        <f t="shared" si="4"/>
+        <v>459.56630365351998</v>
+      </c>
+      <c r="Q57">
+        <f t="shared" si="5"/>
+        <v>2.0791912336241865</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -3704,8 +4148,16 @@
         <f t="shared" si="3"/>
         <v>475.13083749999998</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P58">
+        <f t="shared" si="4"/>
+        <v>462.15736797555104</v>
+      </c>
+      <c r="Q58">
+        <f t="shared" si="5"/>
+        <v>0.94404535863191086</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -3755,8 +4207,16 @@
         <f t="shared" si="3"/>
         <v>475.82875000000001</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P59">
+        <f t="shared" si="4"/>
+        <v>462.50089096260552</v>
+      </c>
+      <c r="Q59">
+        <f t="shared" si="5"/>
+        <v>0.63408768028456564</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -3806,8 +4266,16 @@
         <f t="shared" si="3"/>
         <v>476.87474750000001</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P60">
+        <f t="shared" si="4"/>
+        <v>465.43014341863375</v>
+      </c>
+      <c r="Q60">
+        <f t="shared" si="5"/>
+        <v>0.18576047240634352</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -3857,8 +4325,16 @@
         <f t="shared" si="3"/>
         <v>477.94468499999999</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P61">
+        <f t="shared" si="4"/>
+        <v>466.36606224964601</v>
+      </c>
+      <c r="Q61">
+        <f t="shared" si="5"/>
+        <v>0.32196737453620017</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -3908,8 +4384,16 @@
         <f t="shared" si="3"/>
         <v>479.16979500000002</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P62">
+        <f t="shared" si="4"/>
+        <v>467.54727211006752</v>
+      </c>
+      <c r="Q62">
+        <f t="shared" si="5"/>
+        <v>0.48211519284208748</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -3959,8 +4443,16 @@
         <f t="shared" si="3"/>
         <v>480.47079000000002</v>
       </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P63">
+        <f t="shared" si="4"/>
+        <v>467.20852267483576</v>
+      </c>
+      <c r="Q63">
+        <f t="shared" si="5"/>
+        <v>0.42843299435837423</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -4010,8 +4502,16 @@
         <f t="shared" si="3"/>
         <v>481.920435</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P64">
+        <f t="shared" si="4"/>
+        <v>475.02891057390741</v>
+      </c>
+      <c r="Q64">
+        <f t="shared" si="5"/>
+        <v>0.33673199629349426</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -4061,8 +4561,16 @@
         <f t="shared" si="3"/>
         <v>483.45997499999999</v>
       </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P65">
+        <f t="shared" si="4"/>
+        <v>476.73283914013274</v>
+      </c>
+      <c r="Q65">
+        <f t="shared" si="5"/>
+        <v>0.16579734129793167</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -4112,8 +4620,16 @@
         <f t="shared" si="3"/>
         <v>485.11340749999999</v>
       </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P66">
+        <f t="shared" si="4"/>
+        <v>479.9971165615093</v>
+      </c>
+      <c r="Q66">
+        <f t="shared" si="5"/>
+        <v>1.3397850577860027E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -4148,23 +4664,31 @@
         <v>1947.43595</v>
       </c>
       <c r="L67">
-        <f t="shared" ref="L67:L97" si="4">G67/H67*100</f>
+        <f t="shared" ref="L67:L97" si="6">G67/H67*100</f>
         <v>4.2530013275689003</v>
       </c>
       <c r="M67">
-        <f t="shared" ref="M67:M97" si="5">J67/I67*100</f>
+        <f t="shared" ref="M67:M97" si="7">J67/I67*100</f>
         <v>3.906781372867993</v>
       </c>
       <c r="N67">
-        <f t="shared" ref="N67:N97" si="6">L67-M67</f>
+        <f t="shared" ref="N67:N97" si="8">L67-M67</f>
         <v>0.34621995470090727</v>
       </c>
       <c r="O67">
-        <f t="shared" ref="O67:O97" si="7">K67/4</f>
+        <f t="shared" ref="O67:O97" si="9">K67/4</f>
         <v>486.85898750000001</v>
       </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P67">
+        <f t="shared" ref="P67:P97" si="10">B67/4</f>
+        <v>482.24230679486442</v>
+      </c>
+      <c r="Q67">
+        <f t="shared" si="5"/>
+        <v>0.42726311035812614</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -4199,23 +4723,31 @@
         <v>1954.6157499999999</v>
       </c>
       <c r="L68">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.0765532407113181</v>
       </c>
       <c r="M68">
+        <f t="shared" si="7"/>
+        <v>3.8586392077994525</v>
+      </c>
+      <c r="N68">
+        <f t="shared" si="8"/>
+        <v>0.21791403291186562</v>
+      </c>
+      <c r="O68">
+        <f t="shared" si="9"/>
+        <v>488.65393749999998</v>
+      </c>
+      <c r="P68">
+        <f t="shared" si="10"/>
+        <v>483.69719182464428</v>
+      </c>
+      <c r="Q68">
         <f t="shared" si="5"/>
-        <v>3.8586392077994525</v>
-      </c>
-      <c r="N68">
-        <f t="shared" si="6"/>
-        <v>0.21791403291186562</v>
-      </c>
-      <c r="O68">
-        <f t="shared" si="7"/>
-        <v>488.65393749999998</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.35">
+        <v>0.31833233208394063</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -4250,23 +4782,31 @@
         <v>1961.71046</v>
       </c>
       <c r="L69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.9571706500677228</v>
       </c>
       <c r="M69">
+        <f t="shared" si="7"/>
+        <v>3.8525305708321431</v>
+      </c>
+      <c r="N69">
+        <f t="shared" si="8"/>
+        <v>0.10464007923557972</v>
+      </c>
+      <c r="O69">
+        <f t="shared" si="9"/>
+        <v>490.427615</v>
+      </c>
+      <c r="P69">
+        <f t="shared" si="10"/>
+        <v>484.77483846686584</v>
+      </c>
+      <c r="Q69">
         <f t="shared" si="5"/>
-        <v>3.8525305708321431</v>
-      </c>
-      <c r="N69">
-        <f t="shared" si="6"/>
-        <v>0.10464007923557972</v>
-      </c>
-      <c r="O69">
-        <f t="shared" si="7"/>
-        <v>490.427615</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.35">
+        <v>0.15280189705153191</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -4301,23 +4841,31 @@
         <v>1969.31062</v>
       </c>
       <c r="L70">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.8587625780231138</v>
       </c>
       <c r="M70">
+        <f t="shared" si="7"/>
+        <v>3.8447116221839965</v>
+      </c>
+      <c r="N70">
+        <f t="shared" si="8"/>
+        <v>1.4050955839117307E-2</v>
+      </c>
+      <c r="O70">
+        <f t="shared" si="9"/>
+        <v>492.32765499999999</v>
+      </c>
+      <c r="P70">
+        <f t="shared" si="10"/>
+        <v>490.36002729230694</v>
+      </c>
+      <c r="Q70">
         <f t="shared" si="5"/>
-        <v>3.8447116221839965</v>
-      </c>
-      <c r="N70">
-        <f t="shared" si="6"/>
-        <v>1.4050955839117307E-2</v>
-      </c>
-      <c r="O70">
-        <f t="shared" si="7"/>
-        <v>492.32765499999999</v>
-      </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.35">
+        <v>0.10587738692409232</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -4352,23 +4900,31 @@
         <v>1977.65751</v>
       </c>
       <c r="L71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.7541571056899627</v>
       </c>
       <c r="M71">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.8544038835342604</v>
       </c>
       <c r="N71">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.1002467778442977</v>
       </c>
       <c r="O71">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>494.4143775</v>
       </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P71">
+        <f t="shared" si="10"/>
+        <v>496.9926060371028</v>
+      </c>
+      <c r="Q71">
+        <f t="shared" ref="Q71:Q97" si="11">F71/F67*100-100</f>
+        <v>-7.350369539247481E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -4403,23 +4959,31 @@
         <v>1985.71703</v>
       </c>
       <c r="L72">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.7045164998973932</v>
       </c>
       <c r="M72">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.0147119126354163</v>
       </c>
       <c r="N72">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.31019541273802309</v>
       </c>
       <c r="O72">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>496.42925750000001</v>
       </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P72">
+        <f t="shared" si="10"/>
+        <v>501.20877492706984</v>
+      </c>
+      <c r="Q72">
+        <f t="shared" si="11"/>
+        <v>-0.11768526205683827</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -4454,23 +5018,31 @@
         <v>1998.2604100000001</v>
       </c>
       <c r="L73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.7519650995332929</v>
       </c>
       <c r="M73">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.1605550768554016</v>
       </c>
       <c r="N73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.40858997732210867</v>
       </c>
       <c r="O73">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>499.56510250000002</v>
       </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P73">
+        <f t="shared" si="10"/>
+        <v>504.82011642742015</v>
+      </c>
+      <c r="Q73">
+        <f t="shared" si="11"/>
+        <v>0.16998472161080258</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -4505,23 +5077,31 @@
         <v>2007.52189</v>
       </c>
       <c r="L74">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.8453094397184668</v>
       </c>
       <c r="M74">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.2748578218226774</v>
       </c>
       <c r="N74">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.42954838210421054</v>
       </c>
       <c r="O74">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>501.8804725</v>
       </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P74">
+        <f t="shared" si="10"/>
+        <v>508.12355158570318</v>
+      </c>
+      <c r="Q74">
+        <f t="shared" si="11"/>
+        <v>0.84723363387297468</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -4556,23 +5136,31 @@
         <v>2016.5584899999999</v>
       </c>
       <c r="L75">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.8396925142642298</v>
       </c>
       <c r="M75">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.3475559195005076</v>
       </c>
       <c r="N75">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.50786340523627782</v>
       </c>
       <c r="O75">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>504.13962249999997</v>
       </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P75">
+        <f t="shared" si="10"/>
+        <v>513.80328309662002</v>
+      </c>
+      <c r="Q75">
+        <f t="shared" si="11"/>
+        <v>0.73488194617408453</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -4607,23 +5195,31 @@
         <v>2027.18523</v>
       </c>
       <c r="L76">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.8971812425647943</v>
       </c>
       <c r="M76">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.315982332032883</v>
       </c>
       <c r="N76">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.41880108946808869</v>
       </c>
       <c r="O76">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>506.79630750000001</v>
       </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P76">
+        <f t="shared" si="10"/>
+        <v>511.91901172864976</v>
+      </c>
+      <c r="Q76">
+        <f t="shared" si="11"/>
+        <v>1.4847906858814781</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -4658,23 +5254,31 @@
         <v>2037.83086</v>
       </c>
       <c r="L77">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.7878700338942868</v>
       </c>
       <c r="M77">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.2517730325387815</v>
       </c>
       <c r="N77">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.46390299864449469</v>
       </c>
       <c r="O77">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>509.45771500000001</v>
       </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P77">
+        <f t="shared" si="10"/>
+        <v>515.78370560653116</v>
+      </c>
+      <c r="Q77">
+        <f t="shared" si="11"/>
+        <v>1.1756321188155709</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -4709,23 +5313,31 @@
         <v>2047.9069199999999</v>
       </c>
       <c r="L78">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.6657910780792129</v>
       </c>
       <c r="M78">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.2008828899861452</v>
       </c>
       <c r="N78">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.53509181190693234</v>
       </c>
       <c r="O78">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>511.97672999999998</v>
       </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P78">
+        <f t="shared" si="10"/>
+        <v>518.42463920113994</v>
+      </c>
+      <c r="Q78">
+        <f t="shared" si="11"/>
+        <v>0.48521791112892743</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -4760,23 +5372,31 @@
         <v>2059.49325</v>
       </c>
       <c r="L79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.5616764601107334</v>
       </c>
       <c r="M79">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.156696772144544</v>
       </c>
       <c r="N79">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.59502031203381067</v>
       </c>
       <c r="O79">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>514.8733125</v>
       </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P79">
+        <f t="shared" si="10"/>
+        <v>521.03045634711827</v>
+      </c>
+      <c r="Q79">
+        <f t="shared" si="11"/>
+        <v>0.9664436600482702</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -4811,23 +5431,31 @@
         <v>2068.0679</v>
       </c>
       <c r="L80">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.4736079873409813</v>
       </c>
       <c r="M80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.1033960281901729</v>
       </c>
       <c r="N80">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.6297880408491916</v>
       </c>
       <c r="O80">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>517.016975</v>
       </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P80">
+        <f t="shared" si="10"/>
+        <v>524.1677393997885</v>
+      </c>
+      <c r="Q80">
+        <f t="shared" si="11"/>
+        <v>0.69154306941759103</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -4862,23 +5490,31 @@
         <v>2079.4666999999999</v>
       </c>
       <c r="L81">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.459335725457279</v>
       </c>
       <c r="M81">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.0449868862785436</v>
       </c>
       <c r="N81">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.58565116082126467</v>
       </c>
       <c r="O81">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>519.86667499999999</v>
       </c>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P81">
+        <f t="shared" si="10"/>
+        <v>526.78502766154008</v>
+      </c>
+      <c r="Q81">
+        <f t="shared" si="11"/>
+        <v>0.69624388957825545</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -4913,23 +5549,31 @@
         <v>2088.9252799999999</v>
       </c>
       <c r="L82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.3831213336712898</v>
       </c>
       <c r="M82">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.9981963923839277</v>
       </c>
       <c r="N82">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.6150750587126379</v>
       </c>
       <c r="O82">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>522.23131999999998</v>
       </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P82">
+        <f t="shared" si="10"/>
+        <v>530.03852394421824</v>
+      </c>
+      <c r="Q82">
+        <f t="shared" si="11"/>
+        <v>1.1326116718584984</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -4964,23 +5608,31 @@
         <v>2097.8122899999998</v>
       </c>
       <c r="L83">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.3325647994903078</v>
       </c>
       <c r="M83">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.9534250502319623</v>
       </c>
       <c r="N83">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.62086025074165452</v>
       </c>
       <c r="O83">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>524.45307249999996</v>
       </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P83">
+        <f t="shared" si="10"/>
+        <v>533.90116598581596</v>
+      </c>
+      <c r="Q83">
+        <f t="shared" si="11"/>
+        <v>0.72384054273648246</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -5015,23 +5667,31 @@
         <v>2105.8855400000002</v>
       </c>
       <c r="L84">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.3965835142615872</v>
       </c>
       <c r="M84">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.9164465983727683</v>
       </c>
       <c r="N84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.5198630841111811</v>
       </c>
       <c r="O84">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>526.47138500000005</v>
       </c>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P84">
+        <f t="shared" si="10"/>
+        <v>535.92302253554669</v>
+      </c>
+      <c r="Q84">
+        <f t="shared" si="11"/>
+        <v>0.40907676737722909</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -5066,23 +5726,31 @@
         <v>2113.5398599999999</v>
       </c>
       <c r="L85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.4514286665297038</v>
       </c>
       <c r="M85">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.8805516787420551</v>
       </c>
       <c r="N85">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.42912301221235127</v>
       </c>
       <c r="O85">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>528.38496499999997</v>
       </c>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P85">
+        <f t="shared" si="10"/>
+        <v>534.74955889013154</v>
+      </c>
+      <c r="Q85">
+        <f t="shared" si="11"/>
+        <v>0.65555323514914221</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -5117,23 +5785,31 @@
         <v>2118.0178000000001</v>
       </c>
       <c r="L86">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.5164810335504497</v>
       </c>
       <c r="M86">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.8434184281310637</v>
       </c>
       <c r="N86">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.32693739458061399</v>
       </c>
       <c r="O86">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>529.50445000000002</v>
       </c>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P86">
+        <f t="shared" si="10"/>
+        <v>531.05127907062229</v>
+      </c>
+      <c r="Q86">
+        <f t="shared" si="11"/>
+        <v>0.56300575374052642</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -5168,23 +5844,31 @@
         <v>2122.3657800000001</v>
       </c>
       <c r="L87">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.9974567317322593</v>
       </c>
       <c r="M87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.8449206077187501</v>
       </c>
       <c r="N87">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.1525361240135092</v>
       </c>
       <c r="O87">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>530.59144500000002</v>
       </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P87">
+        <f t="shared" si="10"/>
+        <v>498.79702318537954</v>
+      </c>
+      <c r="Q87">
+        <f t="shared" si="11"/>
+        <v>-7.1475422751632323E-3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -5219,23 +5903,31 @@
         <v>2131.09256</v>
       </c>
       <c r="L88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.5512441598450772</v>
       </c>
       <c r="M88">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.7894961375756804</v>
       </c>
       <c r="N88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.76174802226939686</v>
       </c>
       <c r="O88">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>532.77314000000001</v>
       </c>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P88">
+        <f t="shared" si="10"/>
+        <v>529.19458142561541</v>
+      </c>
+      <c r="Q88">
+        <f t="shared" si="11"/>
+        <v>0.42163822075306712</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -5270,23 +5962,31 @@
         <v>2139.7611099999999</v>
       </c>
       <c r="L89">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.2678014630152337</v>
       </c>
       <c r="M89">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.737485891731934</v>
       </c>
       <c r="N89">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.53031557128329965</v>
       </c>
       <c r="O89">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>534.94027749999998</v>
       </c>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P89">
+        <f t="shared" si="10"/>
+        <v>531.55082542210812</v>
+      </c>
+      <c r="Q89">
+        <f t="shared" si="11"/>
+        <v>0.35414478654391246</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -5321,23 +6021,31 @@
         <v>2147.9298399999998</v>
       </c>
       <c r="L90">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.2137974459940422</v>
       </c>
       <c r="M90">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.6890736395265029</v>
       </c>
       <c r="N90">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.52472380646753924</v>
       </c>
       <c r="O90">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>536.98245999999995</v>
       </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P90">
+        <f t="shared" si="10"/>
+        <v>530.37218920336727</v>
+      </c>
+      <c r="Q90">
+        <f t="shared" si="11"/>
+        <v>0.566252806204389</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -5372,23 +6080,31 @@
         <v>2158.2878900000001</v>
       </c>
       <c r="L91">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.7037591646039885</v>
       </c>
       <c r="M91">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.6166085383415125</v>
       </c>
       <c r="N91">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>8.7150626262475939E-2</v>
       </c>
       <c r="O91">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>539.57197250000002</v>
       </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P91">
+        <f t="shared" si="10"/>
+        <v>542.64864190856315</v>
+      </c>
+      <c r="Q91">
+        <f t="shared" si="11"/>
+        <v>1.7429078916493239</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -5423,23 +6139,31 @@
         <v>2165.4307600000002</v>
       </c>
       <c r="L92">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.0765743779694028</v>
       </c>
       <c r="M92">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.5346601846741508</v>
       </c>
       <c r="N92">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.45808580670474797</v>
       </c>
       <c r="O92">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>541.35769000000005</v>
       </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P92">
+        <f t="shared" si="10"/>
+        <v>549.07812761296475</v>
+      </c>
+      <c r="Q92">
+        <f t="shared" si="11"/>
+        <v>2.0186712290901028</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>92</v>
       </c>
@@ -5474,23 +6198,31 @@
         <v>2174.1989699999999</v>
       </c>
       <c r="L93">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.5331168334195313</v>
       </c>
       <c r="M93">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.4394848607538804</v>
       </c>
       <c r="N93">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.90636802733434907</v>
       </c>
       <c r="O93">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>543.54974249999998</v>
       </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P93">
+        <f t="shared" si="10"/>
+        <v>555.07370970993315</v>
+      </c>
+      <c r="Q93">
+        <f t="shared" si="11"/>
+        <v>3.4606642166649522</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -5525,23 +6257,31 @@
         <v>2181.7535600000001</v>
       </c>
       <c r="L94">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.3266001920402486</v>
       </c>
       <c r="M94">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.3785443248039817</v>
       </c>
       <c r="N94">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-1.0519441327637331</v>
       </c>
       <c r="O94">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>545.43839000000003</v>
       </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P94">
+        <f t="shared" si="10"/>
+        <v>555.64946056679969</v>
+      </c>
+      <c r="Q94">
+        <f t="shared" si="11"/>
+        <v>5.5958336521490679</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>94</v>
       </c>
@@ -5576,23 +6316,31 @@
         <v>2192.76271</v>
       </c>
       <c r="L95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.1526115346429395</v>
       </c>
       <c r="M95">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.3188116577555222</v>
       </c>
       <c r="N95">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-1.1662001231125827</v>
       </c>
       <c r="O95">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>548.19067749999999</v>
       </c>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P95">
+        <f t="shared" si="10"/>
+        <v>553.88134561282368</v>
+      </c>
+      <c r="Q95">
+        <f t="shared" si="11"/>
+        <v>5.6762798877321643</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -5627,23 +6375,31 @@
         <v>2205.8731400000001</v>
       </c>
       <c r="L96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.1007238236865073</v>
       </c>
       <c r="M96">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.2671725544864825</v>
       </c>
       <c r="N96">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-1.1664487307999751</v>
       </c>
       <c r="O96">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>551.46828500000004</v>
       </c>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P96">
+        <f t="shared" si="10"/>
+        <v>555.55090381440903</v>
+      </c>
+      <c r="Q96">
+        <f t="shared" si="11"/>
+        <v>4.5535863488638881</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>96</v>
       </c>
@@ -5678,20 +6434,28 @@
         <v>2217.7811499999998</v>
       </c>
       <c r="L97">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.149051144256684</v>
       </c>
       <c r="M97">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.2227073467708758</v>
       </c>
       <c r="N97">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-1.0736562025141918</v>
       </c>
       <c r="O97">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>554.44528749999995</v>
+      </c>
+      <c r="P97">
+        <f t="shared" si="10"/>
+        <v>557.82594142201594</v>
+      </c>
+      <c r="Q97">
+        <f t="shared" si="11"/>
+        <v>3.6535686488876422</v>
       </c>
     </row>
   </sheetData>

</xml_diff>